<commit_message>
2016 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -148,9 +148,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Panthers</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>Chargers</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1188,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E1" s="20" t="s">
         <v>13</v>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="D4" s="50" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F4" s="43"/>
       <c r="G4" s="44"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D5" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="54" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F5" s="45"/>
       <c r="G5" s="46"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Panthers at Broncos (Game 1).</v>
+        <v>Please pick a winner (V or H) for Jets at Bills (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D6" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="54" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F6" s="45"/>
       <c r="G6" s="46"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Broncos (Game 1).</v>
+        <v>Please assign a weight to the Bills (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="D7" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="54" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F7" s="45"/>
       <c r="G7" s="46"/>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D8" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="54" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F8" s="45"/>
       <c r="G8" s="46"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D9" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="54" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F9" s="45"/>
       <c r="G9" s="46"/>
@@ -1524,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D10" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="45"/>
       <c r="G10" s="46"/>
@@ -1568,7 +1568,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="F11" s="45"/>
       <c r="G11" s="46"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D12" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12" s="45"/>
       <c r="G12" s="46"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D13" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="54" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F13" s="45"/>
       <c r="G13" s="46"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D14" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="54" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F14" s="45"/>
       <c r="G14" s="46"/>
@@ -1714,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D15" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="54" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F15" s="45"/>
       <c r="G15" s="46"/>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D16" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="54" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F16" s="45"/>
       <c r="G16" s="46"/>
@@ -1793,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D17" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="F17" s="45"/>
       <c r="G17" s="46"/>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="52" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D18" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F18" s="45"/>
       <c r="G18" s="46"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="55" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D19" s="56" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F19" s="47"/>
       <c r="G19" s="48"/>

</xml_diff>

<commit_message>
2016 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\2016 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2016 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -166,7 +166,7 @@
     <t>Chargers</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1236,13 +1236,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1282,13 +1282,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Jets at Bills (Game 1).</v>
+        <v>Please pick a winner (V or H) for Texans at Patriots (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1328,13 +1328,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Bills (Game 1).</v>
+        <v>Please assign a weight to the Patriots (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1371,13 +1371,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1414,13 +1414,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1457,13 +1457,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1500,13 +1500,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1538,13 +1538,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1731,13 +1731,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1807,13 +1807,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1845,13 +1845,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2016 Week 2 Final update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -173,7 +173,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -185,13 +185,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -257,6 +250,19 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,10 +555,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -574,156 +580,156 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="13" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1161,29 +1167,29 @@
     <col min="63" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" s="56" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="57" t="s">
+    <row r="1" spans="2:42" s="51" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="59"/>
-      <c r="AE1" s="58"/>
-      <c r="AP1" s="58"/>
-    </row>
-    <row r="2" spans="2:42" s="12" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41"/>
-      <c r="C2" s="42" t="s">
+      <c r="G1" s="54"/>
+      <c r="AE1" s="53"/>
+      <c r="AP1" s="53"/>
+    </row>
+    <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="55"/>
+      <c r="C2" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
       <c r="I2" s="13" t="str">
         <f ca="1">IF(COUNTIF($AA$3:$AD$3,"&gt;0"),"Input Form Error:","")</f>
         <v>Input Form Error:</v>
@@ -1191,21 +1197,21 @@
       <c r="AE2" s="14"/>
       <c r="AP2" s="14"/>
     </row>
-    <row r="3" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+    <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48" t="s">
+      <c r="D3" s="42"/>
+      <c r="E3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="49" t="s">
+      <c r="F3" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="45" t="s">
         <v>11</v>
       </c>
       <c r="H3" s="3"/>
@@ -1877,7 +1883,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
@@ -1893,17 +1899,17 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="51"/>
-      <c r="C21" s="52" t="s">
+    <row r="21" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="46"/>
+      <c r="C21" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="50"/>
       <c r="I21" s="20"/>
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
2016 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>VISITOR</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Jaguars</t>
   </si>
   <si>
-    <t>Eagles</t>
-  </si>
-  <si>
     <t>Lions</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>Browns</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Panthers</t>
   </si>
   <si>
@@ -160,13 +154,16 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Chargers</t>
   </si>
   <si>
-    <t>3</t>
+    <t/>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Packers, Eagles</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1242,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1288,13 +1285,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1318,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Texans at Patriots (Game 1).</v>
+        <v>Please pick a winner (V or H) for Dolphins at Bengals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1334,13 +1331,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1361,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Patriots (Game 1).</v>
+        <v>Please assign a weight to the Bengals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1374,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1417,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1460,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1503,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1579,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1617,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1664,7 +1661,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1772,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1810,16 +1807,16 @@
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="37">
         <f ca="1">IF(ISTEXT($C18),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1848,16 +1845,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(ISTEXT($C19),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1905,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1973,7 +1970,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1982,7 +1979,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2055,7 +2052,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2121,7 +2118,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17301"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>VISITOR</t>
   </si>
@@ -94,19 +94,10 @@
     <t>Redskins</t>
   </si>
   <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Lions</t>
   </si>
   <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
   </si>
   <si>
     <t>Texans</t>
@@ -116,9 +107,6 @@
   </si>
   <si>
     <t>Falcons</t>
-  </si>
-  <si>
-    <t>Saints</t>
   </si>
   <si>
     <t>Browns</t>
@@ -160,10 +148,16 @@
     <t/>
   </si>
   <si>
-    <t>4</t>
+    <t>Eagles</t>
   </si>
   <si>
-    <t>Packers, Eagles</t>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Jaguars, Chiefs, Saints, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1239,13 +1233,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1285,13 +1279,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1318,7 +1312,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Dolphins at Bengals (Game 1).</v>
+        <v>Please pick a winner (V or H) for Cardinals at 49ers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1331,13 +1325,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1361,7 +1355,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Bengals (Game 1).</v>
+        <v>Please assign a weight to the 49ers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1374,13 +1368,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1417,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1466,7 +1460,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1503,13 +1497,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1541,13 +1535,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1579,13 +1573,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1617,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1655,13 +1649,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1693,13 +1687,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1734,13 +1728,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1767,29 +1761,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1810,13 +1804,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1845,16 +1839,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1902,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1970,7 +1964,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1979,7 +1973,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2056,7 +2050,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2122,7 +2116,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>VISITOR</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Jets</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
     <t>Raiders</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>Panthers</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
   </si>
   <si>
     <t>Bills</t>
@@ -154,10 +148,22 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>5</t>
+    <t>Jaguars</t>
   </si>
   <si>
-    <t>Jaguars, Chiefs, Saints, Seahawks</t>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Vikings, Buccaneers</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1233,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1279,13 +1285,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1312,7 +1318,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Cardinals at 49ers (Game 1).</v>
+        <v>Please pick a winner (V or H) for Broncos at Chargers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1325,13 +1331,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1355,7 +1361,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the 49ers (Game 1).</v>
+        <v>Please assign a weight to the Chargers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1368,13 +1374,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1411,13 +1417,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1454,13 +1460,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1497,13 +1503,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1535,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1579,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1611,13 +1617,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1649,13 +1655,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1687,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1728,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1761,29 +1767,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1804,13 +1810,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1839,16 +1845,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1896,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1964,7 +1970,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1973,7 +1979,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2050,7 +2056,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2116,7 +2122,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -79,9 +79,6 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>Bengals</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
   </si>
   <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t>Panthers</t>
   </si>
   <si>
     <t>Bills</t>
@@ -160,10 +154,16 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Vikings</t>
   </si>
   <si>
-    <t>Vikings, Buccaneers</t>
+    <t>Buccaneers</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Panthers, Cowboys</t>
   </si>
 </sst>
 </file>
@@ -1239,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1285,13 +1285,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1318,7 +1318,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Broncos at Chargers (Game 1).</v>
+        <v>Please pick a winner (V or H) for Bears at Packers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1331,13 +1331,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Chargers (Game 1).</v>
+        <v>Please assign a weight to the Packers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1374,13 +1374,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1417,13 +1417,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1460,13 +1460,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1503,13 +1503,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1541,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1579,13 +1579,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1617,13 +1617,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1655,13 +1655,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1693,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1734,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1772,13 +1772,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1810,13 +1810,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1848,13 +1848,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2016 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>VISITOR</t>
   </si>
@@ -115,24 +115,6 @@
     <t>Chargers</t>
   </si>
   <si>
-    <t>Ravens</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Steelers</t>
-  </si>
-  <si>
-    <t>Rams</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -160,10 +142,16 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Panthers</t>
   </si>
   <si>
-    <t>Panthers, Cowboys</t>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Ravens, Rams, Dolphins, Giants, Steelers, 49ers</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1157,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1239,13 +1227,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1285,13 +1273,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1318,7 +1306,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Bears at Packers (Game 1).</v>
+        <v>Please pick a winner (V or H) for Jaguars at Titans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1331,13 +1319,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1361,7 +1349,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Packers (Game 1).</v>
+        <v>Please assign a weight to the Titans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1374,13 +1362,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1417,13 +1405,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1460,13 +1448,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1503,13 +1491,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1541,13 +1529,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1579,13 +1567,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1617,13 +1605,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1655,13 +1643,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1693,13 +1681,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1729,29 +1717,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1767,29 +1755,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1810,13 +1798,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1845,16 +1833,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1902,7 +1890,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1970,7 +1958,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1979,7 +1967,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2056,11 +2044,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2122,11 +2110,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -70,31 +70,16 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Patriots</t>
-  </si>
-  <si>
     <t>Jets</t>
   </si>
   <si>
     <t>Raiders</t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
-    <t>Redskins</t>
-  </si>
-  <si>
     <t>Lions</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Texans</t>
   </si>
   <si>
     <t>Colts</t>
@@ -107,9 +92,6 @@
   </si>
   <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Bears</t>
   </si>
   <si>
     <t>Chargers</t>
@@ -148,10 +130,28 @@
     <t>Cowboys</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Steelers</t>
   </si>
   <si>
-    <t>Ravens, Rams, Dolphins, Giants, Steelers, 49ers</t>
+    <t>Ravens</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Cardinals, Bears, Bengals, Texans, Patriots, Redskins</t>
   </si>
 </sst>
 </file>
@@ -1227,13 +1227,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1273,13 +1273,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Jaguars at Titans (Game 1).</v>
+        <v>Please pick a winner (V or H) for Falcons at Buccaneers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1319,13 +1319,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Titans (Game 1).</v>
+        <v>Please assign a weight to the Buccaneers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1362,13 +1362,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1405,13 +1405,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1448,13 +1448,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1491,13 +1491,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1722,13 +1722,13 @@
         <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1760,13 +1760,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1798,13 +1798,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2016 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>VISITOR</t>
   </si>
@@ -73,25 +73,13 @@
     <t>Jets</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Lions</t>
-  </si>
-  <si>
-    <t>Colts</t>
   </si>
   <si>
     <t>Falcons</t>
   </si>
   <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Chargers</t>
@@ -148,10 +136,28 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Texans</t>
   </si>
   <si>
-    <t>Cardinals, Bears, Bengals, Texans, Patriots, Redskins</t>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Redskins</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Bills, Lions, Colts, Raiders</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1163,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1227,7 +1233,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
@@ -1273,13 +1279,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1306,7 +1312,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Falcons at Buccaneers (Game 1).</v>
+        <v>Please pick a winner (V or H) for Browns at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1319,13 +1325,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1349,7 +1355,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Buccaneers (Game 1).</v>
+        <v>Please assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1362,13 +1368,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1405,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1448,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1491,13 +1497,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1529,13 +1535,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1567,13 +1573,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1605,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1643,13 +1649,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1681,13 +1687,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1717,29 +1723,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1760,13 +1766,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1798,13 +1804,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1833,16 +1839,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1890,7 +1896,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1958,7 +1964,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1967,7 +1973,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2048,7 +2054,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2114,7 +2120,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -70,19 +70,7 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Jets</t>
-  </si>
-  <si>
-    <t>Broncos</t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t>Chargers</t>
   </si>
   <si>
     <t/>
@@ -154,10 +142,22 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>Bills, Lions, Colts, Raiders</t>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Falcons, Broncos, Jets, Chargers</t>
   </si>
 </sst>
 </file>
@@ -1233,13 +1233,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1279,13 +1279,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1312,7 +1312,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Browns at Ravens (Game 1).</v>
+        <v>Please pick a winner (V or H) for Saints at Panthers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1325,13 +1325,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1355,7 +1355,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Ravens (Game 1).</v>
+        <v>Please assign a weight to the Panthers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1368,13 +1368,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1411,13 +1411,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1454,13 +1454,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1497,13 +1497,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1535,13 +1535,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1573,13 +1573,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1611,13 +1611,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1649,13 +1649,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1687,13 +1687,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1766,13 +1766,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1804,13 +1804,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1842,13 +1842,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2016 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>VISITOR</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Eagles</t>
@@ -154,10 +151,22 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Falcons</t>
   </si>
   <si>
-    <t>Falcons, Broncos, Jets, Chargers</t>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1172,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1233,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1279,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1312,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Saints at Panthers (Game 1).</v>
+        <v>Please pick a winner (V or H) for Vikings at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1325,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1355,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Panthers (Game 1).</v>
+        <v>Please assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1368,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1411,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1454,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1497,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1535,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1573,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1611,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1649,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1687,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1728,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1761,29 +1770,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1799,29 +1808,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1839,16 +1848,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1896,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1964,7 +1973,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1973,7 +1982,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2046,11 +2055,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2112,11 +2121,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>VISITOR</t>
   </si>
@@ -65,12 +65,6 @@
   </si>
   <si>
     <t>Input Form</t>
-  </si>
-  <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Browns</t>
   </si>
   <si>
     <t>Eagles</t>
@@ -163,10 +157,13 @@
     <t>Jets</t>
   </si>
   <si>
-    <t>12</t>
+    <t/>
   </si>
   <si>
-    <t>None</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Browns, Titans</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1242,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1288,13 +1285,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1318,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Vikings at Lions (Game 1).</v>
+        <v>Please pick a winner (V or H) for Cowboys at Vikings (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1340,7 +1337,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1361,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Lions (Game 1).</v>
+        <v>Please assign a weight to the Vikings (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1374,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1417,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1460,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1503,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1579,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1617,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1658,13 +1655,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1772,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1808,29 +1805,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1848,16 +1845,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1905,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1973,7 +1970,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1982,7 +1979,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2055,7 +2052,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2121,7 +2118,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>VISITOR</t>
   </si>
@@ -157,13 +157,16 @@
     <t>Jets</t>
   </si>
   <si>
-    <t/>
+    <t>Browns</t>
   </si>
   <si>
-    <t>13</t>
+    <t>Titans</t>
   </si>
   <si>
-    <t>Browns, Titans</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1239,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1285,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1318,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Cowboys at Vikings (Game 1).</v>
+        <v>Please pick a winner (V or H) for Raiders at Chiefs (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1331,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1361,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Vikings (Game 1).</v>
+        <v>Please assign a weight to the Chiefs (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1374,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1417,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1466,7 +1469,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1503,7 +1506,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
@@ -1541,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1579,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1617,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1655,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1693,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1734,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1772,13 +1775,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1805,29 +1808,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1845,16 +1848,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1902,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1970,7 +1973,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1979,7 +1982,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2052,7 +2055,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2118,7 +2121,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2016 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -163,10 +163,10 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>14</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1172,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1242,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1288,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Raiders at Chiefs (Game 1).</v>
+        <v>Please pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1334,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Chiefs (Game 1).</v>
+        <v>Please assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1658,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1775,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1813,13 +1813,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1905,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2016 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -166,7 +166,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1242,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1294,7 +1294,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
+        <v>Please pick a winner (V or H) for Giants at Eagles (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1334,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Seahawks (Game 1).</v>
+        <v>Please assign a weight to the Eagles (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1658,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1775,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1813,13 +1813,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2016 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -166,7 +166,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1242,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1288,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Giants at Eagles (Game 1).</v>
+        <v>Please pick a winner (V or H) for Saints at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1334,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Eagles (Game 1).</v>
+        <v>Please assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1658,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1775,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1813,13 +1813,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
Update regular_season_inputs.xlsx with Week 1 games.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2016 Football Pool Page\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2017 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -166,7 +166,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>17</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -1242,13 +1242,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1288,13 +1288,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Please pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Please pick a winner (V or H) for Saints at Falcons (Game 1).</v>
+        <v>Please pick a winner (V or H) for Chiefs at Patriots (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1334,13 +1334,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE("Please assign a weight to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Please assign a weight to the Falcons (Game 1).</v>
+        <v>Please assign a weight to the Patriots (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1377,13 +1377,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1420,13 +1420,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1506,13 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1544,13 +1544,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1582,13 +1582,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1620,13 +1620,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1658,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1696,13 +1696,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1775,13 +1775,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1813,13 +1813,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1851,13 +1851,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -160,9 +160,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>Monday Night Total Points</t>
   </si>
   <si>
@@ -179,6 +176,9 @@
   </si>
   <si>
     <t>Vikings</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1185,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1255,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1301,13 +1301,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chiefs at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for Texans at Bengals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1347,13 +1347,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Patriots (Game 1).</v>
+        <v>Assign a weight to the Bengals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1390,13 +1390,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1433,13 +1433,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1476,13 +1476,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,13 +1519,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1557,13 +1557,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1595,13 +1595,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1633,13 +1633,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1671,13 +1671,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1709,13 +1709,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1750,13 +1750,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1788,13 +1788,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1826,13 +1826,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1864,13 +1864,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1927,24 +1927,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>

</xml_diff>

<commit_message>
2017 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -178,7 +178,7 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1255,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1301,13 +1301,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Texans at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for Rams at 49ers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1347,13 +1347,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bengals (Game 1).</v>
+        <v>Assign a weight to the 49ers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1390,13 +1390,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1433,13 +1433,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1476,13 +1476,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,13 +1519,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1557,13 +1557,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1595,13 +1595,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,7 +1639,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1671,13 +1671,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1709,13 +1709,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1750,13 +1750,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1788,13 +1788,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1826,13 +1826,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1864,13 +1864,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -178,7 +178,7 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1255,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1301,13 +1301,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Rams at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for Bears at Packers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1347,13 +1347,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the 49ers (Game 1).</v>
+        <v>Assign a weight to the Packers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1390,13 +1390,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1433,13 +1433,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1476,13 +1476,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,13 +1519,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1557,7 +1557,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
@@ -1595,7 +1595,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
@@ -1633,7 +1633,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
@@ -1671,13 +1671,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1709,13 +1709,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1750,13 +1750,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1788,13 +1788,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1826,13 +1826,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1864,13 +1864,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>VISITOR</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>Redskins</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
@@ -139,13 +136,7 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Chargers</t>
-  </si>
-  <si>
-    <t>Broncos</t>
   </si>
   <si>
     <t>Jets</t>
@@ -155,9 +146,6 @@
   </si>
   <si>
     <t>Titans</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>Monday Night Total Points</t>
@@ -172,13 +160,16 @@
     <t>You can't use the same weight more than once.</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
     <t>Vikings</t>
   </si>
   <si>
-    <t>4</t>
+    <t/>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Falcons, Broncos, Saints, Redskins</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1176,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1255,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1301,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1334,7 +1325,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bears at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for Patriots at Buccaneers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1347,13 +1338,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1377,7 +1368,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Packers (Game 1).</v>
+        <v>Assign a weight to the Buccaneers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1390,13 +1381,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1433,13 +1424,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1476,13 +1467,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,13 +1510,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1557,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1595,13 +1586,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1633,13 +1624,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1671,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1709,13 +1700,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1750,13 +1741,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1783,29 +1774,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1821,29 +1812,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1861,16 +1852,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1918,7 +1909,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1927,24 +1918,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>
@@ -2000,7 +1991,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2009,7 +2000,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2082,11 +2073,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2148,11 +2139,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2017 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -79,16 +79,10 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
     <t>Buccaneers</t>
   </si>
   <si>
     <t>Panthers</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
   </si>
   <si>
     <t>Steelers</t>
@@ -119,12 +113,6 @@
   </si>
   <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Bengals</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Lions</t>
@@ -166,10 +154,22 @@
     <t/>
   </si>
   <si>
-    <t>5</t>
+    <t>Falcons</t>
   </si>
   <si>
-    <t>Falcons, Broncos, Saints, Redskins</t>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Redskins</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Bills, Bengals, Cowboys, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
@@ -1292,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Patriots at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for Eagles at Panthers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1338,13 +1338,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1368,7 +1368,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Buccaneers (Game 1).</v>
+        <v>Assign a weight to the Panthers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1381,13 +1381,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1424,13 +1424,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1467,13 +1467,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1510,13 +1510,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1548,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1586,13 +1586,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1624,13 +1624,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1662,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1700,13 +1700,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1741,13 +1741,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1779,13 +1779,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1817,13 +1817,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1855,13 +1855,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1918,24 +1918,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>

</xml_diff>

<commit_message>
2017 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>VISITOR</t>
   </si>
@@ -103,9 +103,6 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>Texans</t>
-  </si>
-  <si>
     <t>Bears</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Lions</t>
   </si>
   <si>
     <t>Colts</t>
@@ -166,10 +160,22 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>Bills, Bengals, Cowboys, Seahawks</t>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Lions, Texans</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1182,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1246,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1292,13 +1298,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1325,7 +1331,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Eagles at Panthers (Game 1).</v>
+        <v>Pick a winner (V or H) for Chiefs at Raiders (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1338,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1368,7 +1374,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Panthers (Game 1).</v>
+        <v>Assign a weight to the Raiders (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1381,13 +1387,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1424,13 +1430,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1467,13 +1473,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1510,13 +1516,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1548,13 +1554,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1586,13 +1592,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1624,13 +1630,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1662,13 +1668,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1700,13 +1706,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1741,13 +1747,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1774,29 +1780,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1817,13 +1823,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1852,16 +1858,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1909,7 +1915,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1918,24 +1924,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>
@@ -1991,7 +1997,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2000,7 +2006,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2077,7 +2083,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2143,7 +2149,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2017 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>VISITOR</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>Packers</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Chiefs</t>
   </si>
   <si>
@@ -94,19 +88,10 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>49ers</t>
   </si>
   <si>
     <t>Bears</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
   </si>
   <si>
     <t>Patriots</t>
@@ -125,9 +110,6 @@
   </si>
   <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t>Titans</t>
   </si>
   <si>
     <t>Monday Night Total Points</t>
@@ -172,10 +154,16 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Texans</t>
   </si>
   <si>
-    <t>Lions, Texans</t>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Cardinals, Packers, Jaguars, Rams, Giants, Titans</t>
   </si>
 </sst>
 </file>
@@ -1182,7 +1170,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>13</v>
@@ -1252,13 +1240,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1298,13 +1286,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1331,7 +1319,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chiefs at Raiders (Game 1).</v>
+        <v>Pick a winner (V or H) for Dolphins at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1344,13 +1332,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1374,7 +1362,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Raiders (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1387,13 +1375,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1430,13 +1418,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1473,13 +1461,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1516,13 +1504,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1554,13 +1542,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1592,13 +1580,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1630,13 +1618,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1668,13 +1656,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1706,13 +1694,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1742,29 +1730,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1780,29 +1768,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1823,13 +1811,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1858,16 +1846,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1915,7 +1903,7 @@
         <v>3</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1924,24 +1912,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>
@@ -1997,7 +1985,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2006,7 +1994,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2083,11 +2071,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2149,11 +2137,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2017 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -79,9 +79,6 @@
     <t>Panthers</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Ravens</t>
   </si>
   <si>
@@ -91,25 +88,13 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>Bears</t>
-  </si>
-  <si>
-    <t>Patriots</t>
-  </si>
-  <si>
     <t>Colts</t>
   </si>
   <si>
     <t>Raiders</t>
   </si>
   <si>
-    <t>Chargers</t>
-  </si>
-  <si>
     <t>Jets</t>
-  </si>
-  <si>
-    <t>Browns</t>
   </si>
   <si>
     <t>Monday Night Total Points</t>
@@ -122,9 +107,6 @@
   </si>
   <si>
     <t>You can't use the same weight more than once.</t>
-  </si>
-  <si>
-    <t>Vikings</t>
   </si>
   <si>
     <t/>
@@ -160,10 +142,28 @@
     <t>Lions</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Jaguars</t>
   </si>
   <si>
-    <t>Cardinals, Packers, Jaguars, Rams, Giants, Titans</t>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Bears, Browns, Chargers, Vikings, Patriots, Steelers</t>
   </si>
 </sst>
 </file>
@@ -1240,13 +1240,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1286,13 +1286,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1319,7 +1319,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Dolphins at Ravens (Game 1).</v>
+        <v>Pick a winner (V or H) for Bills at Jets (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1332,13 +1332,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Ravens (Game 1).</v>
+        <v>Assign a weight to the Jets (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1418,13 +1418,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1542,13 +1542,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1580,13 +1580,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1618,13 +1618,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1656,13 +1656,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1694,13 +1694,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>2</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1735,13 +1735,13 @@
         <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1773,13 +1773,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1811,13 +1811,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1855,7 +1855,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1912,24 +1912,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>

</xml_diff>

<commit_message>
2017 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2017 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -49,19 +49,10 @@
     <t>Input Form</t>
   </si>
   <si>
-    <t>Eagles</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
     <t>Buccaneers</t>
   </si>
   <si>
     <t>Panthers</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Dolphins</t>
@@ -71,9 +62,6 @@
   </si>
   <si>
     <t>Colts</t>
-  </si>
-  <si>
-    <t>Raiders</t>
   </si>
   <si>
     <t>Jets</t>
@@ -142,12 +130,6 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Bears, Browns, Chargers, Vikings, Patriots, Steelers</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -167,6 +149,30 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Ravens, Chiefs, Raiders, Eagles</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1179,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1185,7 +1191,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1200,22 +1206,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F3" s="44" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G3" s="45" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1245,13 +1251,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1291,13 +1297,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1324,7 +1330,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bills at Jets (Game 1).</v>
+        <v>Pick a winner (V or H) for Seahawks at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1337,13 +1343,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1367,7 +1373,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Jets (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1380,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1423,13 +1429,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1466,13 +1472,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1509,7 +1515,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1547,13 +1553,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1585,13 +1591,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1623,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
@@ -1661,13 +1667,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1699,13 +1705,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1735,15 +1741,15 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
         <v>22</v>
@@ -1751,13 +1757,13 @@
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1778,13 +1784,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1816,13 +1822,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1851,16 +1857,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1908,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1917,24 +1923,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>
@@ -1990,7 +1996,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1999,7 +2005,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2080,7 +2086,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2146,7 +2152,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2017 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -52,19 +52,7 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>Panthers</t>
-  </si>
-  <si>
     <t>Dolphins</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Jets</t>
   </si>
   <si>
     <t>Monday Night Total Points</t>
@@ -169,10 +157,22 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Ravens, Chiefs, Raiders, Eagles</t>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Panthers, Colts, Jets, 49ers</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1206,22 +1206,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="G3" s="45" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>40</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1251,13 +1251,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1297,13 +1297,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Seahawks at Cardinals (Game 1).</v>
+        <v>Pick a winner (V or H) for Titans at Steelers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1343,13 +1343,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cardinals (Game 1).</v>
+        <v>Assign a weight to the Steelers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1386,13 +1386,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1429,13 +1429,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1472,13 +1472,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1515,13 +1515,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1553,13 +1553,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1591,13 +1591,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1629,13 +1629,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1667,13 +1667,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1705,13 +1705,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1784,13 +1784,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1822,13 +1822,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1860,13 +1860,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1923,24 +1923,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>

</xml_diff>

<commit_message>
2017 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>at</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>You can't use the same weight more than once.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Falcons</t>
@@ -169,10 +166,22 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Colts</t>
   </si>
   <si>
-    <t>Panthers, Colts, Jets, 49ers</t>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1191,7 +1200,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1206,22 +1215,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>36</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1251,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1297,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1330,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Titans at Steelers (Game 1).</v>
+        <v>Pick a winner (V or H) for Vikings at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1343,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1373,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Steelers (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1386,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1429,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1472,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1515,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1553,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1591,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1629,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1667,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1705,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1746,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1779,29 +1788,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1817,29 +1826,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1857,16 +1866,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1914,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1996,7 +2005,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2005,7 +2014,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2078,11 +2087,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2144,11 +2153,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2017 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -178,10 +178,10 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>12</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Vikings at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Redskins at Cowboys (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Cowboys (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1606,7 +1606,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1714,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
@@ -1793,7 +1793,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1923,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2017 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -181,7 +181,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>13</t>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Redskins at Cowboys (Game 1).</v>
+        <v>Pick a winner (V or H) for Saints at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cowboys (Game 1).</v>
+        <v>Assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1714,7 +1714,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="241"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -181,7 +181,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Saints at Falcons (Game 1).</v>
+        <v>Pick a winner (V or H) for Broncos at Colts (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Falcons (Game 1).</v>
+        <v>Assign a weight to the Colts (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1444,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1714,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -181,7 +181,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Broncos at Colts (Game 1).</v>
+        <v>Pick a winner (V or H) for Colts at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Colts (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,7 +1676,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
@@ -1714,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2017 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -181,7 +181,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Colts at Ravens (Game 1).</v>
+        <v>Pick a winner (V or H) for Panthers at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Ravens (Game 1).</v>
+        <v>Assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,13 +1793,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,13 +1831,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C7435BA0-4BC8-4D0A-8030-0CE92262165C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{463946F8-1C46-4E82-A14C-161CF1ADF978}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Falcons at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for Ravens at Bengals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Eagles (Game 1).</v>
+        <v>Assign a weight to the Bengals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,7 +1756,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{463946F8-1C46-4E82-A14C-161CF1ADF978}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAAC71-4A4B-478E-8A4C-FF58E8577122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Ravens at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for Jets at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bengals (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAAC71-4A4B-478E-8A4C-FF58E8577122}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C7E17-DC22-42D7-91E9-6590A411C5FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Saints</t>
-  </si>
-  <si>
-    <t>Redskins</t>
   </si>
   <si>
     <t>Broncos</t>
@@ -170,19 +167,19 @@
     <t>Colts</t>
   </si>
   <si>
-    <t>Panthers</t>
-  </si>
-  <si>
     <t>Jets</t>
   </si>
   <si>
     <t>49ers</t>
   </si>
   <si>
-    <t>None</t>
+    <t/>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Panthers, Redskins</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1186,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1201,7 +1198,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1216,22 +1213,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>34</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>35</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1261,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,7 +1304,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1340,7 +1337,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jets at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Vikings at Rams (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1380,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Rams (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1436,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1479,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1598,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1636,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1674,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1712,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1753,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1791,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,29 +1824,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1867,16 +1864,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -2006,7 +2003,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2015,7 +2012,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2088,7 +2085,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2154,7 +2151,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820C7E17-DC22-42D7-91E9-6590A411C5FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB984700-AB06-4565-A3BC-43D66B712590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Input Form</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
   </si>
   <si>
     <t>Dolphins</t>
@@ -134,9 +131,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Bears</t>
-  </si>
-  <si>
     <t>Browns</t>
   </si>
   <si>
@@ -176,10 +170,16 @@
     <t/>
   </si>
   <si>
-    <t>4</t>
+    <t>Panthers</t>
   </si>
   <si>
-    <t>Panthers, Redskins</t>
+    <t>Redskins</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Bears, Buccaneers</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1198,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1213,22 +1213,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>33</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>34</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1258,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1304,13 +1304,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Vikings at Rams (Game 1).</v>
+        <v>Pick a winner (V or H) for Colts at Patriots (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1350,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Rams (Game 1).</v>
+        <v>Assign a weight to the Patriots (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1393,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1436,13 +1436,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1479,13 +1479,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1522,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1560,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1598,13 +1598,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1636,13 +1636,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1674,13 +1674,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1712,13 +1712,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1753,13 +1753,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1791,13 +1791,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1829,13 +1829,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1867,13 +1867,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1930,24 +1930,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>

</xml_diff>

<commit_message>
2018 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB984700-AB06-4565-A3BC-43D66B712590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E39767-C5E4-49FF-9C43-501F55FC2349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>Falcons</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>Texans</t>
-  </si>
-  <si>
-    <t>Lions</t>
   </si>
   <si>
     <t>Jaguars</t>
@@ -176,10 +170,16 @@
     <t>Redskins</t>
   </si>
   <si>
-    <t>5</t>
+    <t>Buccaneers</t>
   </si>
   <si>
-    <t>Bears, Buccaneers</t>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Lions, Saints</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1198,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1213,22 +1213,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="G3" s="45" t="s">
         <v>31</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>33</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1258,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1304,13 +1304,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Colts at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for Eagles at Giants (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1350,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1380,7 +1380,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Patriots (Game 1).</v>
+        <v>Assign a weight to the Giants (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1393,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1436,13 +1436,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1479,13 +1479,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1522,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1560,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1598,13 +1598,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1636,13 +1636,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1674,13 +1674,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1712,13 +1712,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1753,13 +1753,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1791,13 +1791,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1829,13 +1829,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1867,13 +1867,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E39767-C5E4-49FF-9C43-501F55FC2349}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B892FB-AF20-4386-BA3E-7D9EF11307CE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Cowboys</t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
     <t>Texans</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Packers</t>
   </si>
   <si>
     <t>Game</t>
@@ -128,9 +122,6 @@
     <t>Browns</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Chargers</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
   </si>
   <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Raiders</t>
   </si>
   <si>
     <t>Eagles</t>
@@ -176,10 +164,16 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Lions</t>
   </si>
   <si>
-    <t>Lions, Saints</t>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Packers, Raiders, Steelers, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1198,7 +1192,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1213,22 +1207,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="G3" s="45" t="s">
         <v>29</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>31</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1258,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1304,13 +1298,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1337,7 +1331,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Eagles at Giants (Game 1).</v>
+        <v>Pick a winner (V or H) for Broncos at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1356,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1380,7 +1374,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Giants (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1393,13 +1387,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1436,7 +1430,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
@@ -1479,13 +1473,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1522,13 +1516,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1560,13 +1554,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1598,13 +1592,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1636,13 +1630,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1674,13 +1668,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1712,13 +1706,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1753,13 +1747,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1786,29 +1780,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1829,13 +1823,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1864,16 +1858,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1921,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2003,7 +1997,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2012,7 +2006,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2089,7 +2083,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2155,7 +2149,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B892FB-AF20-4386-BA3E-7D9EF11307CE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9FD4F5-801D-428C-8283-F5B0183C6EFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>You can't use the same weight more than once.</t>
   </si>
   <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>Bengals</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
   </si>
   <si>
     <t>Texans</t>
@@ -90,9 +84,6 @@
   </si>
   <si>
     <t>Giants</t>
-  </si>
-  <si>
-    <t>Titans</t>
   </si>
   <si>
     <t>Cardinals</t>
@@ -120,9 +111,6 @@
   </si>
   <si>
     <t>Browns</t>
-  </si>
-  <si>
-    <t>Chargers</t>
   </si>
   <si>
     <t>Vikings</t>
@@ -170,10 +158,22 @@
     <t>Saints</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Seahawks</t>
   </si>
   <si>
-    <t>Packers, Raiders, Steelers, Seahawks</t>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Falcons, Cowboys, Chargers, Titans</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1192,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1207,22 +1207,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="F3" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="G3" s="45" t="s">
         <v>26</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>29</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1252,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1298,13 +1298,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Broncos at Cardinals (Game 1).</v>
+        <v>Pick a winner (V or H) for Dolphins at Texans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1344,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1374,7 +1374,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cardinals (Game 1).</v>
+        <v>Assign a weight to the Texans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1387,13 +1387,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1430,13 +1430,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1473,13 +1473,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1516,13 +1516,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1554,13 +1554,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1592,13 +1592,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1630,13 +1630,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1668,13 +1668,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1706,13 +1706,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1747,13 +1747,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1785,13 +1785,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1823,13 +1823,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1861,13 +1861,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9FD4F5-801D-428C-8283-F5B0183C6EFB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA06E15-2403-4C4C-AACE-6D9C950CCAAB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>at</t>
   </si>
@@ -71,22 +71,10 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
     <t>Texans</t>
   </si>
   <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Rams</t>
-  </si>
-  <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
   </si>
   <si>
     <t>Game</t>
@@ -123,12 +111,6 @@
   </si>
   <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Eagles</t>
-  </si>
-  <si>
-    <t>Colts</t>
   </si>
   <si>
     <t>Jets</t>
@@ -170,10 +152,22 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Falcons</t>
   </si>
   <si>
-    <t>Falcons, Cowboys, Chargers, Titans</t>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Cardinals, Bengals, Colts, Jaguars, Giants, Eagles</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1192,7 +1186,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1207,22 +1201,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="G3" s="45" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>26</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1252,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1298,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1331,7 +1325,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Dolphins at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for Raiders at 49ers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1344,13 +1338,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1374,7 +1368,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Texans (Game 1).</v>
+        <v>Assign a weight to the 49ers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1387,13 +1381,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1430,13 +1424,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1473,13 +1467,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1516,13 +1510,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1554,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1592,13 +1586,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1630,13 +1624,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1668,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1706,13 +1700,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1742,29 +1736,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1785,13 +1779,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1823,13 +1817,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1858,16 +1852,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1915,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1997,7 +1991,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2006,7 +2000,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2087,7 +2081,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2153,7 +2147,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA06E15-2403-4C4C-AACE-6D9C950CCAAB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19BF63-E9AB-4A86-8B53-BAD8681C137F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -65,13 +65,7 @@
     <t>You can't use the same weight more than once.</t>
   </si>
   <si>
-    <t>Broncos</t>
-  </si>
-  <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Texans</t>
   </si>
   <si>
     <t>Rams</t>
@@ -101,13 +95,7 @@
     <t>Browns</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -164,10 +152,28 @@
     <t>Cowboys</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Bengals</t>
   </si>
   <si>
-    <t>Cardinals, Bengals, Colts, Jaguars, Giants, Eagles</t>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Ravens, Broncos, Texans, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1186,7 +1192,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1201,22 +1207,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="G3" s="45" t="s">
         <v>20</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>22</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1246,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1292,13 +1298,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1325,7 +1331,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Raiders at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for Panthers at Steelers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1338,13 +1344,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1368,7 +1374,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the 49ers (Game 1).</v>
+        <v>Assign a weight to the Steelers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1381,13 +1387,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1424,13 +1430,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1467,13 +1473,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1510,13 +1516,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1548,13 +1554,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1586,13 +1592,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1624,13 +1630,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1662,13 +1668,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1700,13 +1706,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1736,29 +1742,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1779,13 +1785,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1817,13 +1823,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1852,16 +1858,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1909,7 +1915,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1991,7 +1997,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2000,7 +2006,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2081,7 +2087,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2147,7 +2153,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A19BF63-E9AB-4A86-8B53-BAD8681C137F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD26D367-F5D7-4385-A364-36A23D3C713E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>at</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Input Form</t>
   </si>
   <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
     <t>Monday Night Total Points</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
   </si>
   <si>
     <t>You can't use the same weight more than once.</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Rams</t>
@@ -92,19 +86,7 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Browns</t>
-  </si>
-  <si>
-    <t>Patriots</t>
-  </si>
-  <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Jets</t>
-  </si>
-  <si>
-    <t>49ers</t>
   </si>
   <si>
     <t/>
@@ -170,10 +152,22 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Ravens, Broncos, Texans, Vikings</t>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Bills, Browns, Dolphins, Patriots, Jets, 49ers</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1174,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1192,7 +1186,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1207,22 +1201,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="E3" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="F3" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="G3" s="45" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>20</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1252,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1298,13 +1292,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1331,7 +1325,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Panthers at Steelers (Game 1).</v>
+        <v>Pick a winner (V or H) for Packers at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1344,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
@@ -1374,7 +1368,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Steelers (Game 1).</v>
+        <v>Assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1387,13 +1381,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1430,13 +1424,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1473,13 +1467,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1516,13 +1510,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1554,13 +1548,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1592,13 +1586,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1630,13 +1624,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1668,13 +1662,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1706,13 +1700,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1742,29 +1736,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1785,13 +1779,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1823,13 +1817,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1858,16 +1852,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1915,7 +1909,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1924,24 +1918,24 @@
     </row>
     <row r="22" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA23" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:42" s="5" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G24" s="6"/>
       <c r="AA24" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G25" s="1"/>
       <c r="AA25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AE25" s="1"/>
       <c r="AP25" s="1"/>
@@ -1997,7 +1991,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2006,7 +2000,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2087,7 +2081,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2153,7 +2147,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD26D367-F5D7-4385-A364-36A23D3C713E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF00DE6-5011-43C0-B47A-4775FEEE302F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -62,9 +62,6 @@
     <t>You can't use the same weight more than once.</t>
   </si>
   <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>Game</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t>Chiefs</t>
   </si>
   <si>
     <t/>
@@ -164,10 +158,28 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>Bills, Browns, Dolphins, Patriots, Jets, 49ers</t>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Chiefs, Rams</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1186,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1186,7 +1198,7 @@
     <row r="2" spans="2:42" s="12" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="55"/>
       <c r="C2" s="56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="57"/>
       <c r="E2" s="58"/>
@@ -1201,22 +1213,22 @@
     </row>
     <row r="3" spans="2:42" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="E3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="45" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>18</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="17" t="str">
@@ -1246,13 +1258,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1292,13 +1304,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1325,7 +1337,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Packers at Seahawks (Game 1).</v>
+        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1338,13 +1350,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1368,7 +1380,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Seahawks (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1381,13 +1393,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1424,13 +1436,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1467,13 +1479,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1510,13 +1522,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1548,13 +1560,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1586,13 +1598,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1624,13 +1636,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1662,13 +1674,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1700,13 +1712,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1736,29 +1748,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1774,29 +1786,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1817,13 +1829,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1852,16 +1864,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1909,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1991,7 +2003,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2000,7 +2012,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2077,11 +2089,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2143,11 +2155,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF00DE6-5011-43C0-B47A-4775FEEE302F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D8F7CD-3DEA-448D-8E09-4CF9AB9916AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Regular Season Input Form'!$B$1:$G$24</definedName>
     <definedName name="Season_total_points">'Regular Season Input Form'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>at</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Panthers</t>
@@ -176,10 +173,16 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>12</t>
+    <t>Rams</t>
   </si>
   <si>
-    <t>Chiefs, Rams</t>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1258,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1304,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1337,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Saints at Cowboys (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1350,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1380,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Cowboys (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1393,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1436,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1479,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1522,7 +1525,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1560,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1598,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1636,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1674,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1712,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1753,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1791,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1824,29 +1827,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1864,16 +1867,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1921,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2003,7 +2006,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2012,7 +2015,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2085,7 +2088,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2151,7 +2154,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2018 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D8F7CD-3DEA-448D-8E09-4CF9AB9916AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181FDBD9-2F17-4271-85CE-9E744C864606}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -179,10 +179,10 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>13</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -1189,7 +1189,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Saints at Cowboys (Game 1).</v>
+        <v>Pick a winner (V or H) for Jaguars at Titans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cowboys (Game 1).</v>
+        <v>Assign a weight to the Titans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,7 +1439,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
@@ -1482,7 +1482,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1924,7 +1924,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2018 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181FDBD9-2F17-4271-85CE-9E744C864606}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3AB592-B794-461D-939F-662855FF4994}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jaguars at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for Chargers at Chiefs (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Titans (Game 1).</v>
+        <v>Assign a weight to the Chiefs (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3AB592-B794-461D-939F-662855FF4994}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B78DA8-767F-4320-8F45-2537B0AC115F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chargers at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for Giants at Colts (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chiefs (Game 1).</v>
+        <v>Assign a weight to the Colts (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,7 +1756,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2018 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2018 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B78DA8-767F-4320-8F45-2537B0AC115F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3C93A2-8FB7-4FC3-B2A7-EF5B6D5A16E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="9420" windowHeight="4500" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1261,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1307,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Giants at Colts (Game 1).</v>
+        <v>Pick a winner (V or H) for Browns at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1353,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1383,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Colts (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1396,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1439,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1482,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1525,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1601,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1639,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1677,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1715,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1756,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1794,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1832,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1870,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F47B8E7-FF83-46CB-AE1D-CBAB80EE59B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D7D33A-3131-4A5F-807A-28928F914D68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,13 @@
     <definedName name="Season_total_points">'Regular Season Input Form'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -182,7 +189,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1261,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1307,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1340,7 +1347,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Packers at Bears (Game 1).</v>
+        <v>Pick a winner (V or H) for Buccaneers at Panthers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1353,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1383,7 +1390,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bears (Game 1).</v>
+        <v>Assign a weight to the Panthers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1396,13 +1403,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1439,13 +1446,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1482,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1563,13 +1570,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1601,13 +1608,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1639,13 +1646,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1677,13 +1684,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1715,13 +1722,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1756,13 +1763,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1794,13 +1801,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1832,13 +1839,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1870,13 +1877,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D7D33A-3131-4A5F-807A-28928F914D68}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF66944-64CC-4D3B-9DC2-BF9E2206F7AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1268,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1314,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Buccaneers at Panthers (Game 1).</v>
+        <v>Pick a winner (V or H) for Titans at Jaguars (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1360,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Panthers (Game 1).</v>
+        <v>Assign a weight to the Jaguars (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1403,13 +1403,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1446,13 +1446,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1489,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1532,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1570,13 +1570,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1608,13 +1608,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1646,13 +1646,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1684,13 +1684,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1722,13 +1722,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1763,13 +1763,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1801,13 +1801,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1839,13 +1839,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1877,13 +1877,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF66944-64CC-4D3B-9DC2-BF9E2206F7AB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1452800D-4991-42EE-8DBD-90C4673F6C06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -174,22 +174,19 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>Jets</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
     <t>Chiefs</t>
   </si>
   <si>
-    <t>None</t>
+    <t/>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Jets, 49ers</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1268,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1314,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1347,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Titans at Jaguars (Game 1).</v>
+        <v>Pick a winner (V or H) for Eagles at Packers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1360,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1390,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Jaguars (Game 1).</v>
+        <v>Assign a weight to the Packers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1403,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1446,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1489,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1538,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1570,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1608,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1646,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
@@ -1684,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1722,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1763,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1801,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1834,29 +1831,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1874,16 +1871,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -2013,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2022,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2095,7 +2092,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2161,7 +2158,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1452800D-4991-42EE-8DBD-90C4673F6C06}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E258EFEF-0F3A-472F-A634-231270E09549}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Saints</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
     <t>Browns</t>
   </si>
   <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
     <t>Patriots</t>
   </si>
   <si>
@@ -183,10 +177,16 @@
     <t/>
   </si>
   <si>
-    <t>4</t>
+    <t>Jets</t>
   </si>
   <si>
-    <t>Jets, 49ers</t>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Lions, Dolphins</t>
   </si>
 </sst>
 </file>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Eagles at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Packers (Game 1).</v>
+        <v>Assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,7 +1443,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E258EFEF-0F3A-472F-A634-231270E09549}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E7091-ED96-4151-AE20-1CBB9D62DB29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>Bears</t>
-  </si>
-  <si>
     <t>Saints</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
   </si>
   <si>
     <t>Steelers</t>
-  </si>
-  <si>
-    <t>Raiders</t>
   </si>
   <si>
     <t>Packers</t>
@@ -135,9 +129,6 @@
     <t>Jaguars</t>
   </si>
   <si>
-    <t>Colts</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
   </si>
   <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Browns</t>
@@ -183,10 +171,16 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>5</t>
+    <t>Dolphins</t>
   </si>
   <si>
-    <t>Lions, Dolphins</t>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Bills, Bears, Colts, Raiders</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1187,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1259,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1338,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
+        <v>Pick a winner (V or H) for Giants at Patriots (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1351,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1381,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Seahawks (Game 1).</v>
+        <v>Assign a weight to the Patriots (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1394,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1523,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,7 +1561,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
@@ -1605,13 +1599,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1637,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1675,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1713,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1754,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,29 +1787,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1836,13 +1830,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1871,16 +1865,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2004,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2013,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2096,7 +2090,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2162,7 +2156,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E7091-ED96-4151-AE20-1CBB9D62DB29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FA75C1-62EA-46D8-A2A7-9F6B569D9AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,22 +90,13 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Panthers</t>
-  </si>
-  <si>
     <t>Redskins</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
   </si>
   <si>
     <t>Saints</t>
   </si>
   <si>
     <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Steelers</t>
   </si>
   <si>
     <t>Packers</t>
@@ -150,9 +141,6 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>Browns</t>
-  </si>
-  <si>
     <t>Patriots</t>
   </si>
   <si>
@@ -177,10 +165,22 @@
     <t>Lions</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>Bills, Bears, Colts, Raiders</t>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Panthers, Browns, Steelers, Buccaneers</t>
   </si>
 </sst>
 </file>
@@ -1259,13 +1259,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1305,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Giants at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for Chiefs at Broncos (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1351,13 +1351,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Patriots (Game 1).</v>
+        <v>Assign a weight to the Broncos (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1394,13 +1394,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1437,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1523,7 +1523,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1561,13 +1561,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1599,13 +1599,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1637,13 +1637,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1675,13 +1675,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1713,13 +1713,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1754,13 +1754,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1792,13 +1792,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1830,13 +1830,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1868,13 +1868,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FA75C1-62EA-46D8-A2A7-9F6B569D9AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DEDF4B-7D88-495C-8CB1-4DF04909A19A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>Bengals</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
   </si>
   <si>
     <t>Giants</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Vikings</t>
@@ -177,10 +171,22 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Buccaneers</t>
   </si>
   <si>
-    <t>Panthers, Browns, Steelers, Buccaneers</t>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Ravens, Cowboys</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1259,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1305,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1338,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chiefs at Broncos (Game 1).</v>
+        <v>Pick a winner (V or H) for Redskins at Vikings (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1351,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1381,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Broncos (Game 1).</v>
+        <v>Assign a weight to the Vikings (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1394,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1437,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1480,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1523,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1561,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1599,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1637,7 +1643,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
@@ -1675,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1713,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1754,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1787,29 +1793,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1830,13 +1836,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,16 +1871,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2004,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2013,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2090,7 +2096,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2156,7 +2162,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DEDF4B-7D88-495C-8CB1-4DF04909A19A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58971212-54C7-4CB2-818D-23796871EC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -93,25 +93,16 @@
     <t>Redskins</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
     <t>Seahawks</t>
   </si>
   <si>
     <t>Packers</t>
   </si>
   <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Chargers</t>
   </si>
   <si>
     <t>Titans</t>
-  </si>
-  <si>
-    <t>Bengals</t>
   </si>
   <si>
     <t>Jaguars</t>
@@ -136,9 +127,6 @@
   </si>
   <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Rams</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -183,10 +171,16 @@
     <t>Steelers</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Ravens, Cowboys</t>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Falcons, Bengals, Rams, Saints</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1187,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1259,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1305,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1338,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Redskins at Vikings (Game 1).</v>
+        <v>Pick a winner (V or H) for 49ers at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1351,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1381,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Vikings (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1394,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1437,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1523,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1561,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1599,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1637,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1675,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1713,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1754,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,29 +1787,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1836,13 +1830,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1871,16 +1865,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1922,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2004,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2013,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2096,7 +2090,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2162,7 +2156,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58971212-54C7-4CB2-818D-23796871EC1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D09D1DC-4DFD-4406-8FBE-6FB75604E824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
   <si>
     <t>at</t>
   </si>
@@ -90,9 +90,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Redskins</t>
-  </si>
-  <si>
     <t>Seahawks</t>
   </si>
   <si>
@@ -105,28 +102,13 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Eagles</t>
   </si>
   <si>
     <t>Giants</t>
   </si>
   <si>
     <t>Vikings</t>
-  </si>
-  <si>
-    <t>Texans</t>
-  </si>
-  <si>
-    <t>Broncos</t>
-  </si>
-  <si>
-    <t>Patriots</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -177,10 +159,22 @@
     <t>Cowboys</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Bengals</t>
   </si>
   <si>
-    <t>Falcons, Bengals, Rams, Saints</t>
+    <t>Falcons</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Broncos, Texans, Jaguars, Patriots, Eagles, Redskins</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1259,13 +1253,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1305,13 +1299,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1338,7 +1332,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for 49ers at Cardinals (Game 1).</v>
+        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1351,13 +1345,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1381,7 +1375,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cardinals (Game 1).</v>
+        <v>Assign a weight to the Raiders (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1394,13 +1388,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1437,13 +1431,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1480,13 +1474,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1523,13 +1517,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1561,13 +1555,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1599,13 +1593,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1637,13 +1631,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1675,13 +1669,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1713,13 +1707,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1749,29 +1743,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1792,13 +1786,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1830,13 +1824,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,16 +1859,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2004,7 +1998,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2013,7 +2007,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2094,7 +2088,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2160,7 +2154,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D09D1DC-4DFD-4406-8FBE-6FB75604E824}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21151F3-DFCF-40C8-87ED-BBE6917F72B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -90,22 +91,10 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Chargers</t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Giants</t>
   </si>
   <si>
     <t>Vikings</t>
@@ -171,10 +160,28 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Texans</t>
   </si>
   <si>
-    <t>Broncos, Texans, Jaguars, Patriots, Eagles, Redskins</t>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Redskins</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Packers, Giants, Seahawks, Titans</t>
   </si>
 </sst>
 </file>
@@ -1181,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1253,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1299,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1332,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
+        <v>Pick a winner (V or H) for Steelers at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1345,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1375,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Raiders (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1388,13 +1395,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1431,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1474,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1517,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1555,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1593,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1631,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1669,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1707,13 +1714,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1743,29 +1750,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1786,13 +1793,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1824,13 +1831,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1859,16 +1866,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1916,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -1998,7 +2005,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2007,7 +2014,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2088,7 +2095,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2154,7 +2161,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21151F3-DFCF-40C8-87ED-BBE6917F72B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B6EE35-910D-4C0B-95F4-026D74FC097F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,18 +91,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Chargers</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Vikings</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -178,10 +166,22 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Giants</t>
   </si>
   <si>
-    <t>Packers, Giants, Seahawks, Titans</t>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Cardinals, Chiefs, Chargers, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1260,13 +1260,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1306,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Steelers at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Colts at Texans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1352,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Texans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,7 +1395,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
@@ -1438,13 +1438,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1481,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1562,13 +1562,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1600,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1638,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1676,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,13 +1755,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1793,13 +1793,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,13 +1831,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1869,13 +1869,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B6EE35-910D-4C0B-95F4-026D74FC097F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3850B84-941C-48CC-A02F-88D64995E5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>at</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Jets</t>
@@ -178,10 +175,22 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>12</t>
+    <t>Chiefs</t>
   </si>
   <si>
-    <t>Cardinals, Chiefs, Chargers, Vikings</t>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1197,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1266,7 +1275,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1306,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1339,7 +1348,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Colts at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1352,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1382,7 +1391,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Texans (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1395,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1438,13 +1447,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1481,13 +1490,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1524,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1562,13 +1571,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1600,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1638,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1676,13 +1685,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1714,13 +1723,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1755,13 +1764,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1788,29 +1797,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1826,29 +1835,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1866,16 +1875,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1923,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2005,7 +2014,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2014,7 +2023,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2087,11 +2096,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2153,11 +2162,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2019 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3850B84-941C-48CC-A02F-88D64995E5E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F84B5D9-17C6-4B51-81FE-841C1A35CD05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,10 +187,10 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>13</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>14</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1197,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1269,13 +1269,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1315,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Cowboys at Bears (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1361,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Bears (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1404,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1453,7 +1453,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1490,13 +1490,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1533,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1571,13 +1571,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1609,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1647,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1685,13 +1685,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1723,7 +1723,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1764,13 +1764,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,13 +1802,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1840,13 +1840,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1878,13 +1878,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2019 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F84B5D9-17C6-4B51-81FE-841C1A35CD05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A669F-9774-40A1-BE26-C08C3AF5C0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>14</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1269,13 +1269,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1315,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cowboys at Bears (Game 1).</v>
+        <v>Pick a winner (V or H) for Jets at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1361,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bears (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1404,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1447,7 +1447,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
@@ -1496,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1533,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1571,13 +1571,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1609,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1647,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1685,13 +1685,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1723,13 +1723,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1764,13 +1764,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,13 +1802,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1840,13 +1840,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1878,13 +1878,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454A669F-9774-40A1-BE26-C08C3AF5C0F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7352D518-60F2-4432-A9A7-93C9693C29E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1269,13 +1269,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1315,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jets at Ravens (Game 1).</v>
+        <v>Pick a winner (V or H) for Lions at Broncos (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1361,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Ravens (Game 1).</v>
+        <v>Assign a weight to the Broncos (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1404,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1447,13 +1447,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1490,13 +1490,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1533,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1571,13 +1571,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1609,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1647,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1685,13 +1685,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1723,13 +1723,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1764,13 +1764,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,13 +1802,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1840,13 +1840,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1878,13 +1878,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2019 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2019 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7352D518-60F2-4432-A9A7-93C9693C29E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B547D32-835A-4854-B2FF-2B3D7FBFE005}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1269,13 +1269,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1315,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1348,7 +1348,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Lions at Broncos (Game 1).</v>
+        <v>Pick a winner (V or H) for Steelers at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1361,13 +1361,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1391,7 +1391,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Broncos (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1404,13 +1404,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1447,13 +1447,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1490,13 +1490,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1533,13 +1533,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1571,13 +1571,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1609,13 +1609,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1647,13 +1647,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1685,13 +1685,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1723,13 +1723,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1764,13 +1764,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,13 +1802,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1840,13 +1840,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1878,13 +1878,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
Regular season code improvements.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0661F9-F918-493A-9E6A-71CA80D13633}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD43F42E-FF16-4070-BF31-4F1B07E09F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Regular Season Input Form'!$B$1:$G$24</definedName>
-    <definedName name="Season_total_points">'Regular Season Input Form'!#REF!</definedName>
+    <definedName name="current_week">'Regular Season Input Form'!$D$1</definedName>
+    <definedName name="current_week_schedule">'Regular Season Input Form'!$C$4:$E$19</definedName>
+    <definedName name="mn_points">'Regular Season Input Form'!$G$20</definedName>
+    <definedName name="open_date_teams">'Regular Season Input Form'!$D$21</definedName>
+    <definedName name="player_name">'Regular Season Input Form'!$D$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Regular Season Input Form'!$B$1:$G$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>

<commit_message>
Replace "Redskins" with "Football Team"
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD43F42E-FF16-4070-BF31-4F1B07E09F2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDF515-76D2-4F64-B1AF-2246334BDA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Regular Season Input Form'!$B$1:$G$21</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -158,9 +150,6 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>Redskins</t>
-  </si>
-  <si>
     <t>Patriots</t>
   </si>
   <si>
@@ -195,6 +184,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Football Team</t>
   </si>
 </sst>
 </file>
@@ -1180,9 +1172,9 @@
   <cols>
     <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" style="11" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="1" customWidth="1"/>
@@ -1201,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1279,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1319,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1575,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1619,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1651,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1689,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
@@ -1768,7 +1760,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
@@ -1850,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1882,7 +1874,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
@@ -1936,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2020 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBDF515-76D2-4F64-B1AF-2246334BDA5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A0FF6-C3DE-44CF-A613-AB06CA45D09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,10 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
+    <t>Football Team</t>
   </si>
   <si>
-    <t>Football Team</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Texans at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for Bengals at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chiefs (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310A0FF6-C3DE-44CF-A613-AB06CA45D09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB88DCD-172A-4B85-BE53-788133BE9EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -186,7 +186,7 @@
     <t>Football Team</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bengals at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Dolphins at Jaguars (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Jaguars (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1535,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,7 +1567,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
@@ -1605,7 +1605,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,7 +1719,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB88DCD-172A-4B85-BE53-788133BE9EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5EE5A8-DCE6-4D32-BF2E-FB38375A3848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,7 +186,7 @@
     <t>Football Team</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Dolphins at Jaguars (Game 1).</v>
+        <v>Pick a winner (V or H) for Broncos at Jets (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Jaguars (Game 1).</v>
+        <v>Assign a weight to the Jets (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5EE5A8-DCE6-4D32-BF2E-FB38375A3848}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DED04C-58D0-4006-B2BB-36A7497583EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Bills</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Seahawks</t>
   </si>
   <si>
@@ -180,13 +174,16 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Football Team</t>
   </si>
   <si>
-    <t>4</t>
+    <t/>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Lions, Packers</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1190,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1262,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1308,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1341,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Broncos at Jets (Game 1).</v>
+        <v>Pick a winner (V or H) for Buccaneers at Bears (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1354,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1384,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Jets (Game 1).</v>
+        <v>Assign a weight to the Bears (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1397,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1440,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1483,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1526,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1564,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1602,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1640,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1678,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1716,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1757,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1795,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,29 +1828,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1871,16 +1868,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2007,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2016,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2092,7 +2089,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2158,7 +2155,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2020 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667051B5-C2E1-404E-A1B2-74C06C2FF2BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EA2B94-B8D2-471E-B31B-90068EEC114B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>at</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
     <t>Colts</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>Falcons</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
@@ -147,9 +141,6 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>Patriots</t>
-  </si>
-  <si>
     <t>Eagles</t>
   </si>
   <si>
@@ -157,9 +148,6 @@
   </si>
   <si>
     <t>Titans</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -180,10 +168,16 @@
     <t/>
   </si>
   <si>
-    <t>5</t>
+    <t>Lions</t>
   </si>
   <si>
-    <t>Lions, Packers</t>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Patriots, Raiders, Saints, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1184,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1262,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1308,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1341,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Buccaneers at Bears (Game 1).</v>
+        <v>Pick a winner (V or H) for Chiefs at Bills (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1354,13 +1348,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1384,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bears (Game 1).</v>
+        <v>Assign a weight to the Bills (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1397,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1440,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1483,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1526,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1564,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1602,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1640,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1678,13 +1672,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1716,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1757,13 +1751,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1790,29 +1784,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1833,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1868,16 +1862,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1925,7 +1919,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2007,7 +2001,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2016,7 +2010,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2093,7 +2087,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2159,7 +2153,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
NFL schedule update due to Week 5 "Broncos at Patriots" postponement.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5EA2B94-B8D2-471E-B31B-90068EEC114B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3979B9-C33E-4427-AF93-6CE3D1579E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>Patriots, Raiders, Saints, Seahawks</t>
+    <t>Raiders, Saints, Seahawks</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
2020 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3979B9-C33E-4427-AF93-6CE3D1579E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D125A52-DB0B-443C-A787-027AB688DB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -93,13 +93,7 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Colts</t>
   </si>
   <si>
     <t>Bears</t>
@@ -115,9 +109,6 @@
   </si>
   <si>
     <t>Steelers</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Cowboys</t>
@@ -159,9 +150,6 @@
     <t>Chargers</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
     <t>Football Team</t>
   </si>
   <si>
@@ -174,10 +162,22 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Saints</t>
   </si>
   <si>
-    <t>Raiders, Saints, Seahawks</t>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Colts, Dolphins, Ravens, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1256,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1302,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chiefs at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for Giants at Eagles (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1348,13 +1348,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bills (Game 1).</v>
+        <v>Assign a weight to the Eagles (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1434,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1564,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1672,13 +1672,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1751,13 +1751,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1789,13 +1789,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
2020 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D125A52-DB0B-443C-A787-027AB688DB12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E206D-BFC4-4170-9E0C-93C7FC1C40BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -123,12 +123,6 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>Texans</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
@@ -144,13 +138,7 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
     <t>Chargers</t>
-  </si>
-  <si>
-    <t>Football Team</t>
   </si>
   <si>
     <t/>
@@ -174,10 +162,22 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Colts, Dolphins, Ravens, Vikings</t>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Cardinals, Football Team, Jaguars, Texans</t>
   </si>
 </sst>
 </file>
@@ -1256,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Giants at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for Falcons at Panthers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Eagles (Game 1).</v>
+        <v>Assign a weight to the Panthers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,7 +1391,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
@@ -1440,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1558,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1751,13 +1751,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1789,13 +1789,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,13 +1865,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E206D-BFC4-4170-9E0C-93C7FC1C40BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C0132-360D-4D72-AAB7-D5546147FC76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,28 +105,16 @@
     <t>Panthers</t>
   </si>
   <si>
-    <t>Browns</t>
-  </si>
-  <si>
     <t>Steelers</t>
   </si>
   <si>
     <t>Cowboys</t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
     <t>Falcons</t>
   </si>
   <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Eagles</t>
   </si>
   <si>
     <t>Giants</t>
@@ -174,10 +162,22 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Texans</t>
   </si>
   <si>
-    <t>Cardinals, Football Team, Jaguars, Texans</t>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Football Team</t>
+  </si>
+  <si>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Bengals, Browns, Eagles, Rams</t>
   </si>
 </sst>
 </file>
@@ -1256,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1302,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Falcons at Panthers (Game 1).</v>
+        <v>Pick a winner (V or H) for Packers at 49ers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1348,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Panthers (Game 1).</v>
+        <v>Assign a weight to the 49ers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1434,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1558,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1672,13 +1672,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1751,13 +1751,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1789,13 +1789,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,13 +1865,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296C0132-360D-4D72-AAB7-D5546147FC76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784829D4-3E02-45CC-B151-EDC5CCF79B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Jets</t>
-  </si>
-  <si>
     <t>49ers</t>
   </si>
   <si>
@@ -108,12 +105,6 @@
     <t>Steelers</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
   </si>
   <si>
     <t>Titans</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
   </si>
   <si>
     <t>Chargers</t>
@@ -174,10 +162,22 @@
     <t>Cardinals</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Browns</t>
   </si>
   <si>
-    <t>Bengals, Browns, Eagles, Rams</t>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Chiefs, Cowboys, Falcons, Jets</t>
   </si>
 </sst>
 </file>
@@ -1256,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1302,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Packers at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for Colts at Titans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1348,13 +1348,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the 49ers (Game 1).</v>
+        <v>Assign a weight to the Titans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1434,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1558,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1672,13 +1672,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1757,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1789,13 +1789,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1871,7 +1871,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784829D4-3E02-45CC-B151-EDC5CCF79B79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4CE22C-C9D4-435D-8AE6-A073237C7786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -87,15 +87,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>49ers</t>
-  </si>
-  <si>
-    <t>Bills</t>
-  </si>
-  <si>
-    <t>Bears</t>
-  </si>
-  <si>
     <t>Buccaneers</t>
   </si>
   <si>
@@ -106,9 +97,6 @@
   </si>
   <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Giants</t>
   </si>
   <si>
     <t>Titans</t>
@@ -174,10 +162,22 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Falcons</t>
   </si>
   <si>
-    <t>Chiefs, Cowboys, Falcons, Jets</t>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>49ers, Bears, Bills, Giants</t>
   </si>
 </sst>
 </file>
@@ -1256,13 +1256,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1302,13 +1302,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1335,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Colts at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for Cardinals at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1348,13 +1348,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Titans (Game 1).</v>
+        <v>Assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1434,13 +1434,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1477,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1520,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1558,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1596,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1634,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1672,13 +1672,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,13 +1710,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1751,13 +1751,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1789,13 +1789,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1827,13 +1827,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1865,13 +1865,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4CE22C-C9D4-435D-8AE6-A073237C7786}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A39A09-FB3E-4CAB-AA78-4AE3934BB671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>at</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Chargers</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Lions</t>
   </si>
   <si>
@@ -174,10 +171,22 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>49ers, Bears, Bills, Giants</t>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1256,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1302,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1335,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cardinals at Seahawks (Game 1).</v>
+        <v>Pick a winner (V or H) for Texans at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1348,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1378,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Seahawks (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1391,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1434,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1477,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1520,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1558,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1596,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1634,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1672,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1710,7 +1719,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1751,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1784,29 +1793,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1822,29 +1831,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1862,16 +1871,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1919,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2001,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2010,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2083,11 +2092,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2149,11 +2158,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2020 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A39A09-FB3E-4CAB-AA78-4AE3934BB671}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7CDB83-E790-49EF-B05D-D784A03FE3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -85,12 +85,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
-  </si>
-  <si>
-    <t>Panthers</t>
   </si>
   <si>
     <t>Steelers</t>
@@ -183,10 +177,13 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>12</t>
+    <t/>
   </si>
   <si>
-    <t>None</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Buccaneers, Panthers</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1190,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1262,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1308,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1341,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Texans at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Cowboys at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1354,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1384,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1406,7 +1403,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1440,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1483,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1526,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1564,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1602,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1640,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1678,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1716,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1757,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1795,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1831,29 +1828,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1871,16 +1868,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2007,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2016,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2092,7 +2089,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2158,7 +2155,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2020 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7CDB83-E790-49EF-B05D-D784A03FE3B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37AD75-6EA1-4D35-8499-E17FCA64CAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>at</t>
   </si>
@@ -177,13 +177,16 @@
     <t>Bears</t>
   </si>
   <si>
-    <t/>
+    <t>Panthers</t>
   </si>
   <si>
-    <t>13</t>
+    <t>Buccaneers</t>
   </si>
   <si>
-    <t>Buccaneers, Panthers</t>
+    <t>14</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1190,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1262,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1308,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1341,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cowboys at Ravens (Game 1).</v>
+        <v>Pick a winner (V or H) for Patriots at Rams (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1354,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
@@ -1384,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Ravens (Game 1).</v>
+        <v>Assign a weight to the Rams (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1397,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1440,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1483,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1526,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1564,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1602,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1640,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1678,7 +1681,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
@@ -1716,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1757,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1795,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1828,29 +1831,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1868,16 +1871,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1925,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2007,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2016,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2089,7 +2092,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2155,7 +2158,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2020 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF37AD75-6EA1-4D35-8499-E17FCA64CAC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE0738-FB0D-4D2D-AC89-94B8826764DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -183,10 +183,10 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>14</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Patriots at Rams (Game 1).</v>
+        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Rams (Game 1).</v>
+        <v>Assign a weight to the Raiders (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2020 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EE0738-FB0D-4D2D-AC89-94B8826764DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10DD88-D6BF-4916-8FAE-FCBBD705AA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,7 +186,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>15</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
+        <v>Pick a winner (V or H) for Vikings at Saints (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Raiders (Game 1).</v>
+        <v>Assign a weight to the Saints (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,7 +1719,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2020 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2020 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B10DD88-D6BF-4916-8FAE-FCBBD705AA81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AEBBC3-E4E1-4FD9-B3BC-69909D9B7E1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -186,7 +186,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1265,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1311,13 +1311,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Vikings at Saints (Game 1).</v>
+        <v>Pick a winner (V or H) for Dolphins at Bills (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1357,13 +1357,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$23," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Saints (Game 1).</v>
+        <v>Assign a weight to the Bills (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1400,13 +1400,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1443,13 +1443,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1486,13 +1486,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1529,13 +1529,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1567,13 +1567,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1605,13 +1605,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1643,13 +1643,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1681,13 +1681,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1719,13 +1719,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1760,13 +1760,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1798,13 +1798,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1836,13 +1836,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,13 +1874,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FC29D9-2CB0-4EBD-B76B-B3D08AE46BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9818F553-70BB-457E-960F-A36BCFC82982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cowboys at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for Giants at Football Team (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Buccaneers (Game 1).</v>
+        <v>Assign a weight to the Football Team (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Ravens at Raiders (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Lions at Packers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9818F553-70BB-457E-960F-A36BCFC82982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76919F8C-0D23-4AA9-BFB1-19F7525DBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Giants at Football Team (Game 1).</v>
+        <v>Pick a winner (V or H) for Panthers at Texans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Football Team (Game 1).</v>
+        <v>Assign a weight to the Texans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Lions at Packers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Eagles at Cowboys (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76919F8C-0D23-4AA9-BFB1-19F7525DBA7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B1860F-07E8-473A-8B5A-E02966DCD5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Panthers at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for Jaguars at Bengals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Texans (Game 1).</v>
+        <v>Assign a weight to the Bengals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Eagles at Cowboys (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Raiders at Chargers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B1860F-07E8-473A-8B5A-E02966DCD5BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F03D333-0364-47B8-BD3E-651FFE12E62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,7 +1320,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jaguars at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bengals (Game 1).</v>
+        <v>Assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Raiders at Chargers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Colts at Ravens (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,7 +1538,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F03D333-0364-47B8-BD3E-651FFE12E62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EB1FEC-7050-42BE-A70B-C12F1CE863C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,11 +25,20 @@
     <definedName name="total_points">'Regular Season Input Form'!$G$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -103,9 +112,6 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>Saints</t>
-  </si>
-  <si>
     <t>Seahawks</t>
   </si>
   <si>
@@ -151,13 +157,7 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>Falcons</t>
-  </si>
-  <si>
     <t>Cowboys</t>
-  </si>
-  <si>
-    <t>Jets</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -169,9 +169,6 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Bears</t>
   </si>
   <si>
@@ -181,10 +178,13 @@
     <t>Buccaneers</t>
   </si>
   <si>
-    <t>None</t>
+    <t/>
   </si>
   <si>
-    <t>5</t>
+    <t>6</t>
+  </si>
+  <si>
+    <t>49ers, Falcons, Jets, Saints</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Rams at Seahawks (Game 1).</v>
+        <v>Pick a winner (V or H) for Buccaneers at Eagles (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Seahawks (Game 1).</v>
+        <v>Assign a weight to the Eagles (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Colts at Ravens (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bills at Titans (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,29 +1802,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1840,29 +1840,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1880,16 +1880,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1922,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2025,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2098,11 +2098,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2164,11 +2164,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EB1FEC-7050-42BE-A70B-C12F1CE863C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A441609C-3B68-4BAD-9D9A-375DAD3034AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>at</t>
   </si>
@@ -94,16 +94,10 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
     <t>Titans</t>
-  </si>
-  <si>
-    <t>Chargers</t>
   </si>
   <si>
     <t>Lions</t>
@@ -127,16 +121,10 @@
     <t>Colts</t>
   </si>
   <si>
-    <t>Vikings</t>
-  </si>
-  <si>
     <t>Dolphins</t>
   </si>
   <si>
     <t>Texans</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
   </si>
   <si>
     <t>Football Team</t>
@@ -157,13 +145,7 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Bills</t>
   </si>
   <si>
     <t>Giants</t>
@@ -181,10 +163,22 @@
     <t/>
   </si>
   <si>
-    <t>6</t>
+    <t>Falcons</t>
   </si>
   <si>
-    <t>49ers, Falcons, Jets, Saints</t>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Bills, Chargers, Cowboys, Jaguars, Steelers, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1196,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1347,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Buccaneers at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for Broncos at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1390,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Eagles (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1403,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1446,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1519,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bills at Titans (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Saints at Seahawks (Game 13) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1570,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1608,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1646,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1684,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1722,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1764,29 +1758,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1807,13 +1801,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1839,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1880,16 +1874,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1916,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 13 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2106,7 +2100,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2172,7 +2166,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A441609C-3B68-4BAD-9D9A-375DAD3034AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95D441B-248B-4D62-BC47-087C9873354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -112,12 +112,6 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
-    <t>Ravens</t>
-  </si>
-  <si>
     <t>Colts</t>
   </si>
   <si>
@@ -175,10 +169,28 @@
     <t>Saints</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Bills</t>
   </si>
   <si>
-    <t>Bills, Chargers, Cowboys, Jaguars, Steelers, Vikings</t>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Raiders, Ravens</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1268,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1314,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1347,7 +1359,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Broncos at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Packers at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1360,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1390,7 +1402,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1446,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1489,13 +1501,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,7 +1531,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Saints at Seahawks (Game 13) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Giants at Chiefs (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1532,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1570,13 +1582,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1608,13 +1620,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1646,13 +1658,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1684,13 +1696,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1722,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1758,29 +1770,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1796,29 +1808,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1839,13 +1851,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,16 +1886,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1916,7 +1928,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 13 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1931,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2022,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2031,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2096,11 +2108,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2162,11 +2174,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95D441B-248B-4D62-BC47-087C9873354D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170B98B-082E-4136-B3B0-9359AD2C0BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -100,13 +100,7 @@
     <t>Titans</t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Packers</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
   </si>
   <si>
     <t>Patriots</t>
@@ -119,9 +113,6 @@
   </si>
   <si>
     <t>Texans</t>
-  </si>
-  <si>
-    <t>Football Team</t>
   </si>
   <si>
     <t>Cardinals</t>
@@ -149,9 +140,6 @@
   </si>
   <si>
     <t>Panthers</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
   </si>
   <si>
     <t/>
@@ -187,10 +175,16 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Raiders, Ravens</t>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Buccaneers, Football Team, Lions, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1280,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1359,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Packers at Cardinals (Game 1).</v>
+        <v>Pick a winner (V or H) for Jets at Colts (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1372,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1402,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cardinals (Game 1).</v>
+        <v>Assign a weight to the Colts (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1415,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1458,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1501,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1531,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Giants at Chiefs (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bears at Steelers (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1544,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1582,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1620,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1658,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1696,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1734,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1775,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1808,29 +1802,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1851,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1886,16 +1880,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1922,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1943,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2022,7 +2016,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2031,7 +2025,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2108,7 +2102,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2174,7 +2168,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0170B98B-082E-4136-B3B0-9359AD2C0BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415027-61EF-4D2F-900E-F59D2D6FC884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Texans</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
@@ -124,19 +121,10 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
     <t>Rams</t>
   </si>
   <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Bears</t>
   </si>
   <si>
     <t>Panthers</t>
@@ -181,10 +169,22 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Lions</t>
   </si>
   <si>
-    <t>Buccaneers, Football Team, Lions, Seahawks</t>
+    <t>Buccaneers</t>
+  </si>
+  <si>
+    <t>Football Team</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Bears, Bengals, Giants, Texans</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jets at Colts (Game 1).</v>
+        <v>Pick a winner (V or H) for Ravens at Dolphins (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Colts (Game 1).</v>
+        <v>Assign a weight to the Dolphins (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bears at Steelers (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at 49ers (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34415027-61EF-4D2F-900E-F59D2D6FC884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4C7B3E-0ABA-40E7-9C5B-5CBE7A09E85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -94,9 +94,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Broncos</t>
-  </si>
-  <si>
     <t>Titans</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>Eagles</t>
-  </si>
-  <si>
-    <t>Rams</t>
   </si>
   <si>
     <t>Chiefs</t>
@@ -181,10 +175,22 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Bears</t>
   </si>
   <si>
-    <t>Bears, Bengals, Giants, Texans</t>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Broncos, Rams</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1359,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Ravens at Dolphins (Game 1).</v>
+        <v>Pick a winner (V or H) for Patriots at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1402,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Dolphins (Game 1).</v>
+        <v>Assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1415,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,7 +1501,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
@@ -1525,7 +1531,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Rams at 49ers (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Giants at Buccaneers (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1582,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1620,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1658,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1696,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1775,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,29 +1808,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1845,13 +1851,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1880,16 +1886,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1928,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2022,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2031,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2102,7 +2108,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2168,7 +2174,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4C7B3E-0ABA-40E7-9C5B-5CBE7A09E85B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D6843-27CF-45AF-ACA6-FF0B52E59139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -109,16 +109,10 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
     <t>Browns</t>
   </si>
   <si>
     <t>Eagles</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
   </si>
   <si>
     <t>Panthers</t>
@@ -187,10 +181,16 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Broncos</t>
   </si>
   <si>
-    <t>Broncos, Rams</t>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Cardinals, Chiefs</t>
   </si>
 </sst>
 </file>
@@ -1280,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Patriots at Falcons (Game 1).</v>
+        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1372,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Falcons (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1415,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
@@ -1458,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1501,13 +1501,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Giants at Buccaneers (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Seahawks at Football Team (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1544,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1582,13 +1582,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1620,13 +1620,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1658,13 +1658,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1696,13 +1696,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1734,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1775,13 +1775,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1813,13 +1813,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1851,13 +1851,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1889,13 +1889,13 @@
         <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495D6843-27CF-45AF-ACA6-FF0B52E59139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B974EBE-C000-4DCC-B562-EFB7938A097B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -94,12 +94,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t>Patriots</t>
   </si>
   <si>
@@ -109,13 +103,7 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Browns</t>
-  </si>
-  <si>
     <t>Eagles</t>
-  </si>
-  <si>
-    <t>Panthers</t>
   </si>
   <si>
     <t/>
@@ -187,10 +175,16 @@
     <t>Rams</t>
   </si>
   <si>
-    <t>12</t>
+    <t>Cardinals</t>
   </si>
   <si>
-    <t>Cardinals, Chiefs</t>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Browns, Packers, Panthers, Titans</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1280,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1359,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bears at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Cowboys at Saints (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1372,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1402,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Saints (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1415,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1458,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1501,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1531,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Seahawks at Football Team (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Patriots at Bills (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1544,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1582,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1620,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1658,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1696,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1734,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1775,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1808,29 +1802,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1851,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1886,16 +1880,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1922,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1943,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2022,7 +2016,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2031,7 +2025,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2108,7 +2102,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2174,7 +2168,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B974EBE-C000-4DCC-B562-EFB7938A097B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2141504-2B5D-4294-98F1-09217B1477D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,18 +94,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Patriots</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Eagles</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -181,10 +169,22 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>13</t>
+    <t>Panthers</t>
   </si>
   <si>
-    <t>Browns, Packers, Panthers, Titans</t>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Colts, Dolphins, Eagles, Patriots</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cowboys at Saints (Game 1).</v>
+        <v>Pick a winner (V or H) for Steelers at Vikings (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Saints (Game 1).</v>
+        <v>Assign a weight to the Vikings (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1415,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Patriots at Bills (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at Cardinals (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2141504-2B5D-4294-98F1-09217B1477D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C6561-B2F9-4B3D-B00D-6D6D765D4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Falcons</t>
@@ -181,10 +178,22 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>14</t>
+    <t>Patriots</t>
   </si>
   <si>
-    <t>Colts, Dolphins, Eagles, Patriots</t>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Steelers at Vikings (Game 1).</v>
+        <v>Pick a winner (V or H) for Chiefs at Chargers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Vikings (Game 1).</v>
+        <v>Assign a weight to the Chargers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Rams at Cardinals (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Vikings at Bears (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,29 +1811,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1840,29 +1849,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1880,16 +1889,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1931,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2025,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2034,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2098,11 +2107,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2164,11 +2173,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2021 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C6561-B2F9-4B3D-B00D-6D6D765D4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D938AB40-76D3-436A-8113-3126458CCF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,10 +190,10 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>15</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chiefs at Chargers (Game 1).</v>
+        <v>Pick a winner (V or H) for 49ers at Titans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chargers (Game 1).</v>
+        <v>Assign a weight to the Titans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Vikings at Bears (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Dolphins at Saints (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1946,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>

</xml_diff>

<commit_message>
2021 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D938AB40-76D3-436A-8113-3126458CCF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2F2498-E150-4126-AA68-B228445331B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for 49ers at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for Falcons at Bills (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Titans (Game 1).</v>
+        <v>Assign a weight to the Bills (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Dolphins at Saints (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Browns at Steelers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2021 Week 17 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2021 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2F2498-E150-4126-AA68-B228445331B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C46FCD-1A2C-4157-AC9D-08FA9948FE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Falcons at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for Saints at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bills (Game 1).</v>
+        <v>Assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Browns at Steelers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Chargers at Raiders (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D77CC2-7BC2-4638-B945-22C91D8ABF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2374E9F-969E-4B5C-AEFC-2508C3403564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bills at Rams (Game 1).</v>
+        <v>Pick a winner (V or H) for Chargers at Chiefs (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Rams (Game 1).</v>
+        <v>Assign a weight to the Chiefs (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Broncos at Seahawks (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Vikings at Eagles (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1591,7 +1591,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2374E9F-969E-4B5C-AEFC-2508C3403564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FDFC49-43A6-4F74-A5D6-2CA4C88AF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chargers at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for Steelers at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chiefs (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Vikings at Eagles (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Cowboys at Giants (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FDFC49-43A6-4F74-A5D6-2CA4C88AF1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B30CF5C-EC32-4588-A53F-85E403754688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Steelers at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Dolphins at Bengals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Bengals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Cowboys at Giants (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at 49ers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B30CF5C-EC32-4588-A53F-85E403754688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C2EA6-6CE0-41DA-A240-B00794C0EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -1283,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Dolphins at Bengals (Game 1).</v>
+        <v>Pick a winner (V or H) for Colts at Broncos (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bengals (Game 1).</v>
+        <v>Assign a weight to the Broncos (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Rams at 49ers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Raiders at Chiefs (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,7 +1737,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1778,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1816,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1854,13 +1854,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1892,13 +1892,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206C2EA6-6CE0-41DA-A240-B00794C0EE1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA6706-8465-49B2-A7C1-A3B1C116A9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -127,12 +127,6 @@
     <t>Ravens</t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Buccaneers</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
   </si>
   <si>
     <t>Bears</t>
-  </si>
-  <si>
-    <t>Texans</t>
   </si>
   <si>
     <t>Bengals</t>
@@ -169,9 +160,6 @@
     <t>Browns</t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
     <t>Packers</t>
   </si>
   <si>
@@ -187,13 +175,16 @@
     <t>Eagles</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Commanders</t>
   </si>
   <si>
-    <t>5</t>
+    <t/>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Lions, Raiders, Texans, Titans</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1283,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Colts at Broncos (Game 1).</v>
+        <v>Pick a winner (V or H) for Commanders at Bears (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Broncos (Game 1).</v>
+        <v>Assign a weight to the Bears (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Raiders at Chiefs (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Broncos at Chargers (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1778,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1811,29 +1802,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1849,29 +1840,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1889,16 +1880,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1931,7 +1922,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1946,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2025,7 +2016,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2034,7 +2025,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2107,11 +2098,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2173,11 +2164,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CA6706-8465-49B2-A7C1-A3B1C116A9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2AD72-9D63-486F-B9C0-C7DD2FDD1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Saints</t>
   </si>
   <si>
-    <t>Bills</t>
-  </si>
-  <si>
     <t>Steelers</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
   </si>
   <si>
     <t>Cowboys</t>
-  </si>
-  <si>
-    <t>Vikings</t>
   </si>
   <si>
     <t>Ravens</t>
@@ -143,9 +137,6 @@
   </si>
   <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Rams</t>
   </si>
   <si>
     <t>Cardinals</t>
@@ -172,19 +163,28 @@
     <t>Dolphins</t>
   </si>
   <si>
-    <t>Eagles</t>
-  </si>
-  <si>
     <t>Commanders</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>6</t>
+    <t>Lions</t>
   </si>
   <si>
-    <t>Lions, Raiders, Texans, Titans</t>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Texans</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Bills, Eagles, Rams, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Commanders at Bears (Game 1).</v>
+        <v>Pick a winner (V or H) for Saints at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bears (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Broncos at Chargers (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bears at Patriots (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A2AD72-9D63-486F-B9C0-C7DD2FDD1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C5AC35-4C62-410E-92CE-BA8DB5041CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Steelers</t>
   </si>
   <si>
-    <t>Chargers</t>
-  </si>
-  <si>
     <t>Jaguars</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
   </si>
   <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
   </si>
   <si>
     <t>Panthers</t>
@@ -181,10 +175,22 @@
     <t>Raiders</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Vikings</t>
   </si>
   <si>
-    <t>Bills, Eagles, Rams, Vikings</t>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Chargers, Chiefs</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1359,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Saints at Cardinals (Game 1).</v>
+        <v>Pick a winner (V or H) for Ravens at Buccaneers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1402,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cardinals (Game 1).</v>
+        <v>Assign a weight to the Buccaneers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1415,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1501,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1531,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bears at Patriots (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bengals at Browns (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1582,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1620,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1658,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1696,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1775,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,29 +1808,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1845,13 +1851,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1880,7 +1886,7 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
         <v>29</v>
@@ -1889,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1928,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2022,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2031,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2102,7 +2108,7 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2168,7 +2174,7 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C5AC35-4C62-410E-92CE-BA8DB5041CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF645C-BD70-4BE4-A053-575F471912BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>at</t>
   </si>
@@ -100,19 +100,10 @@
     <t>Jets</t>
   </si>
   <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Saints</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Cowboys</t>
   </si>
   <si>
     <t>Ravens</t>
@@ -130,19 +121,10 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Broncos</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
     <t>Panthers</t>
-  </si>
-  <si>
-    <t>Browns</t>
   </si>
   <si>
     <t>Packers</t>
@@ -187,10 +169,16 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>8</t>
+    <t>Chargers</t>
   </si>
   <si>
-    <t>Chargers, Chiefs</t>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>49ers, Broncos, Browns, Cowboys, Giants, Steelers</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1196,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1280,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1359,7 +1347,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Ravens at Buccaneers (Game 1).</v>
+        <v>Pick a winner (V or H) for Eagles at Texans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1372,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1402,7 +1390,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Buccaneers (Game 1).</v>
+        <v>Assign a weight to the Texans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1421,7 +1409,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1458,13 +1446,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1501,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1531,7 +1519,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bengals at Browns (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Ravens at Saints (Game 13) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1544,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1582,7 +1570,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
@@ -1620,13 +1608,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1658,13 +1646,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1696,13 +1684,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1734,13 +1722,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1770,29 +1758,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1808,29 +1796,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1851,13 +1839,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1886,16 +1874,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1928,7 +1916,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 13 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1943,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2022,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2031,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2108,11 +2096,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2174,11 +2162,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBF645C-BD70-4BE4-A053-575F471912BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679F3556-D6C4-476F-911D-B511005F1995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -97,16 +97,10 @@
     <t>Falcons</t>
   </si>
   <si>
-    <t>Jets</t>
-  </si>
-  <si>
     <t>Saints</t>
   </si>
   <si>
     <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Ravens</t>
   </si>
   <si>
     <t>Buccaneers</t>
@@ -118,9 +112,6 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>Bengals</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
   </si>
   <si>
     <t>Packers</t>
-  </si>
-  <si>
-    <t>Patriots</t>
   </si>
   <si>
     <t>Colts</t>
@@ -175,10 +163,28 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>9</t>
+    <t>Browns</t>
   </si>
   <si>
-    <t>49ers, Broncos, Browns, Cowboys, Giants, Steelers</t>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>Steelers</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>49ers</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Bengals, Jets, Patriots, Ravens</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1202,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1268,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1314,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1347,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Eagles at Texans (Game 1).</v>
+        <v>Pick a winner (V or H) for Falcons at Panthers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1360,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1390,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Texans (Game 1).</v>
+        <v>Assign a weight to the Panthers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1403,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1446,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1489,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Ravens at Saints (Game 13) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Commanders at Eagles (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1532,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1570,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1608,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1646,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1684,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1722,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1758,29 +1764,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1801,13 +1807,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1839,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1874,16 +1880,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1916,7 +1922,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 13 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1931,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2016,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2025,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2100,7 +2106,7 @@
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2166,7 +2172,7 @@
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679F3556-D6C4-476F-911D-B511005F1995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627AB95-1F77-4B91-B61D-1810BCED2B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,15 +100,6 @@
     <t>Saints</t>
   </si>
   <si>
-    <t>Jaguars</t>
-  </si>
-  <si>
-    <t>Buccaneers</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
-  </si>
-  <si>
     <t>Bears</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
   </si>
   <si>
     <t>Colts</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
   </si>
   <si>
     <t>Commanders</t>
@@ -181,10 +169,22 @@
     <t>49ers</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Bengals, Jets, Patriots, Ravens</t>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Buccaneers, Dolphins, Jaguars, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1274,13 +1274,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1320,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Falcons at Panthers (Game 1).</v>
+        <v>Pick a winner (V or H) for Titans at Packers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1366,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Panthers (Game 1).</v>
+        <v>Assign a weight to the Packers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1452,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1495,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1525,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Commanders at Eagles (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for 49ers at Cardinals (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1538,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1576,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1614,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1652,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1690,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1728,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1769,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1807,13 +1807,13 @@
         <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1845,13 +1845,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1883,13 +1883,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>

</xml_diff>

<commit_message>
2022 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627AB95-1F77-4B91-B61D-1810BCED2B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2815E951-5B01-4629-89FF-6D8EAF0EE6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -118,9 +118,6 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Lions</t>
   </si>
   <si>
@@ -181,10 +178,22 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Buccaneers</t>
   </si>
   <si>
-    <t>Buccaneers, Dolphins, Jaguars, Seahawks</t>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Seahawks</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1274,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1320,13 +1329,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1353,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Titans at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for Bills at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1366,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1396,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Packers (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1409,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1452,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1495,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1525,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for 49ers at Cardinals (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Steelers at Colts (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1538,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1576,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1614,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1652,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1690,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1728,13 +1737,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1769,13 +1778,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1802,29 +1811,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1840,29 +1849,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1880,16 +1889,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1922,7 +1931,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1937,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2016,7 +2025,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2025,7 +2034,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2098,11 +2107,11 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2164,11 +2173,11 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2815E951-5B01-4629-89FF-6D8EAF0EE6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2652C813-0D6C-409D-8550-8C980EF52C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -101,12 +101,6 @@
   </si>
   <si>
     <t>Bears</t>
-  </si>
-  <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Panthers</t>
   </si>
   <si>
     <t>Packers</t>
@@ -190,10 +184,13 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t>12</t>
+    <t/>
   </si>
   <si>
-    <t>None</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Cardinals, Panthers</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1208,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1283,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1329,13 +1326,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1362,7 +1359,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bills at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Bills at Patriots (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1375,13 +1372,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1405,7 +1402,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Patriots (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1418,13 +1415,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1461,13 +1458,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1504,13 +1501,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1534,7 +1531,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Steelers at Colts (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Saints at Buccaneers (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1547,13 +1544,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1585,13 +1582,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1623,13 +1620,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1661,13 +1658,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1699,13 +1696,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1737,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1784,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
@@ -1816,13 +1813,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
@@ -1849,29 +1846,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37">
+      <c r="B18" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1889,16 +1886,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1931,7 +1928,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1946,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2025,7 +2022,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2034,7 +2031,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2107,7 +2104,7 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2173,7 +2170,7 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2652C813-0D6C-409D-8550-8C980EF52C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F77C09-006B-4F0B-9440-7F24DB9B8691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>at</t>
   </si>
@@ -92,24 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
-    <t>Saints</t>
-  </si>
-  <si>
-    <t>Bears</t>
-  </si>
-  <si>
-    <t>Packers</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Commanders</t>
   </si>
   <si>
     <t>Lions</t>
@@ -187,10 +169,16 @@
     <t/>
   </si>
   <si>
-    <t>13</t>
+    <t>Panthers</t>
   </si>
   <si>
-    <t>Cardinals, Panthers</t>
+    <t>Cardinals</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Bears, Colts, Commanders, Falcons, Packers, Saints</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1196,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1280,13 +1268,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1326,13 +1314,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="24"/>
@@ -1359,7 +1347,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bills at Patriots (Game 1).</v>
+        <v>Pick a winner (V or H) for Raiders at Rams (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1372,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1402,7 +1390,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Patriots (Game 1).</v>
+        <v>Assign a weight to the Rams (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1415,13 +1403,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1458,13 +1446,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1501,13 +1489,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1531,7 +1519,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Saints at Buccaneers (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Patriots at Cardinals (Game 13) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1544,13 +1532,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1582,13 +1570,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1620,13 +1608,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1658,13 +1646,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1696,13 +1684,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1734,13 +1722,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="24"/>
@@ -1770,29 +1758,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37">
+      <c r="B16" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="30" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1808,29 +1796,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37">
+      <c r="B17" s="37" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="30" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1851,13 +1839,13 @@
         <v/>
       </c>
       <c r="C18" s="30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
@@ -1886,10 +1874,10 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
@@ -1928,7 +1916,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 13 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1943,7 +1931,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2022,7 +2010,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2031,7 +2019,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2108,11 +2096,11 @@
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2174,11 +2162,11 @@
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F77C09-006B-4F0B-9440-7F24DB9B8691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C53399-60EA-4DA6-9FBE-76113772E69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regular Season Input Form" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -166,19 +166,34 @@
     <t>Seahawks</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Panthers</t>
   </si>
   <si>
     <t>Cardinals</t>
   </si>
   <si>
-    <t>14</t>
+    <t>Colts</t>
   </si>
   <si>
-    <t>Bears, Colts, Commanders, Falcons, Packers, Saints</t>
+    <t>Falcons</t>
+  </si>
+  <si>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Commanders</t>
+  </si>
+  <si>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1211,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="51" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E1" s="53" t="s">
         <v>7</v>
@@ -1268,13 +1283,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F4" s="21"/>
       <c r="G4" s="22"/>
@@ -1314,7 +1329,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>0</v>
@@ -1347,7 +1362,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Raiders at Rams (Game 1).</v>
+        <v>Pick a winner (V or H) for 49ers at Seahawks (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1360,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="32" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="24"/>
@@ -1390,7 +1405,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Rams (Game 1).</v>
+        <v>Assign a weight to the Seahawks (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1403,13 +1418,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="24"/>
@@ -1446,13 +1461,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="32" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="24"/>
@@ -1489,13 +1504,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="24"/>
@@ -1519,7 +1534,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Patriots at Cardinals (Game 13) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at Packers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1532,13 +1547,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="32" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F10" s="23"/>
       <c r="G10" s="24"/>
@@ -1570,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="32" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F11" s="23"/>
       <c r="G11" s="24"/>
@@ -1608,13 +1623,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F12" s="23"/>
       <c r="G12" s="24"/>
@@ -1646,13 +1661,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="32" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F13" s="23"/>
       <c r="G13" s="24"/>
@@ -1684,13 +1699,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D14" s="31" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="24"/>
@@ -1722,7 +1737,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>0</v>
@@ -1758,29 +1773,29 @@
       </c>
     </row>
     <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="37" t="str">
+      <c r="B16" s="37">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E16" s="32" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="24"/>
       <c r="I16" s="20"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1796,29 +1811,29 @@
       </c>
     </row>
     <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="37" t="str">
+      <c r="B17" s="37">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="24"/>
       <c r="I17" s="20"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1834,29 +1849,29 @@
       </c>
     </row>
     <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="37" t="str">
+      <c r="B18" s="37">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
       <c r="I18" s="20"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1874,16 +1889,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="38">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" s="33" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D19" s="34" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F19" s="25"/>
       <c r="G19" s="26"/>
@@ -1916,7 +1931,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="39" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 13 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="40"/>
       <c r="I20" s="20"/>
@@ -1931,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="48" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E21" s="49"/>
       <c r="F21" s="49"/>
@@ -2010,7 +2025,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -2019,7 +2034,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2092,15 +2107,15 @@
     <row r="40" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="8">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2158,15 +2173,15 @@
     <row r="41" spans="3:42" s="8" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C41" s="8" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="8" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2022 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED22B8B-BB64-48D6-8915-5F185C0F699E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FD1097-9D7C-4481-8D50-267B3683145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1277,13 +1277,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1323,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jaguars at Jets (Game 1).</v>
+        <v>Pick a winner (V or H) for Cowboys at Titans (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1369,13 +1369,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Jets (Game 1).</v>
+        <v>Assign a weight to the Titans (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1412,13 +1412,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1455,13 +1455,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1498,7 +1498,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Chargers at Colts (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bills at Bengals (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1541,13 +1541,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1579,13 +1579,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1617,13 +1617,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1655,13 +1655,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1693,13 +1693,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1731,13 +1731,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1772,13 +1772,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1810,13 +1810,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1848,13 +1848,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1886,13 +1886,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2022 Week 17 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2022 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FD1097-9D7C-4481-8D50-267B3683145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE632B9-6F92-43F0-B2FD-E9E3FEABB983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1277,13 +1277,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1323,13 +1323,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Cowboys at Titans (Game 1).</v>
+        <v>Pick a winner (V or H) for Buccaneers at Falcons (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1369,13 +1369,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1399,7 +1399,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Titans (Game 1).</v>
+        <v>Assign a weight to the Falcons (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1412,13 +1412,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1455,13 +1455,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1498,13 +1498,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bills at Bengals (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at Seahawks (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1541,13 +1541,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1579,13 +1579,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1617,13 +1617,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1655,13 +1655,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1699,7 +1699,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1731,13 +1731,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1772,13 +1772,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1810,13 +1810,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1848,13 +1848,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1886,13 +1886,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 1 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CFA29D-7CB6-4B9F-A979-D4360A0111CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5521FB76-4DBA-46AB-B1B4-E17260411A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -854,9 +854,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -894,9 +894,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -929,26 +929,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -981,26 +964,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1278,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1324,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1357,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Lions at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for Vikings at Eagles (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1370,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1400,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chiefs (Game 1).</v>
+        <v>Assign a weight to the Eagles (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1413,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1456,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1499,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1529,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bills at Jets (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Browns at Steelers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1542,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1580,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1618,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1656,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1694,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1732,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1773,7 +1739,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
@@ -1811,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1849,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1887,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 2 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5521FB76-4DBA-46AB-B1B4-E17260411A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD4C02B-46F0-4A3D-8608-4AD682D791CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>2</t>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Vikings at Eagles (Game 1).</v>
+        <v>Pick a winner (V or H) for Giants at 49ers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Eagles (Game 1).</v>
+        <v>Assign a weight to the 49ers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Browns at Steelers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Rams at Bengals (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1777,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1815,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1853,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 3 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD4C02B-46F0-4A3D-8608-4AD682D791CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5258DD-05B8-4D87-A224-BEEC8A21C7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>3</t>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Giants at 49ers (Game 1).</v>
+        <v>Pick a winner (V or H) for Lions at Packers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the 49ers (Game 1).</v>
+        <v>Assign a weight to the Packers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Rams at Bengals (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Seahawks at Giants (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1777,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1815,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1853,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 4 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5258DD-05B8-4D87-A224-BEEC8A21C7CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AC4ACE-FDBA-4613-A150-EE4668205DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -119,13 +119,7 @@
     <t>Bills</t>
   </si>
   <si>
-    <t>Chargers</t>
-  </si>
-  <si>
     <t>Chiefs</t>
-  </si>
-  <si>
-    <t>Browns</t>
   </si>
   <si>
     <t>Giants</t>
@@ -155,16 +149,10 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>Buccaneers</t>
-  </si>
-  <si>
     <t>Jaguars</t>
   </si>
   <si>
     <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Seahawks</t>
   </si>
   <si>
     <t>Panthers</t>
@@ -191,10 +179,13 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>None</t>
+    <t/>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Browns, Buccaneers, Chargers, Seahawks</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1244,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1281,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1314,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Lions at Packers (Game 1).</v>
+        <v>Pick a winner (V or H) for Bears at Commanders (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1327,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1357,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Packers (Game 1).</v>
+        <v>Assign a weight to the Commanders (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1370,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1456,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1486,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Seahawks at Giants (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Packers at Raiders (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1537,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1575,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1613,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1689,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1730,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1771,30 +1762,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1809,30 +1800,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
+    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1850,16 +1841,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1892,7 +1883,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1907,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1986,7 +1977,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1995,7 +1986,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2073,11 +2064,11 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2141,11 +2132,11 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 5 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AC4ACE-FDBA-4613-A150-EE4668205DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A0BEB-5E94-4A36-863C-EE027A89334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -125,9 +125,6 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>Steelers</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
@@ -176,16 +173,25 @@
     <t>Bears</t>
   </si>
   <si>
-    <t>Packers</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>5</t>
+    <t>Seahawks</t>
   </si>
   <si>
-    <t>Browns, Buccaneers, Chargers, Seahawks</t>
+    <t>Browns</t>
+  </si>
+  <si>
+    <t>Buccaneers</t>
+  </si>
+  <si>
+    <t>Chargers</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Packers, Steelers</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1169,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1235,13 +1241,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1281,13 +1287,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1314,7 +1320,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bears at Commanders (Game 1).</v>
+        <v>Pick a winner (V or H) for Broncos at Chiefs (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1327,13 +1333,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1357,7 +1363,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Commanders (Game 1).</v>
+        <v>Assign a weight to the Chiefs (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1370,13 +1376,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1413,13 +1419,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1456,13 +1462,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1486,7 +1492,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Packers at Raiders (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Cowboys at Chargers (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1499,13 +1505,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1537,13 +1543,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1575,13 +1581,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1613,13 +1619,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1657,7 +1663,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1689,13 +1695,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1730,13 +1736,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1762,30 +1768,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="str">
+    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1806,13 +1812,13 @@
         <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1841,16 +1847,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1883,7 +1889,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1898,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1977,7 +1983,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1986,7 +1992,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2068,7 +2074,7 @@
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2136,7 +2142,7 @@
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 6 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7A0BEB-5E94-4A36-863C-EE027A89334C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D134FE-553B-4457-8AD4-11645E600428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>at</t>
   </si>
@@ -98,12 +98,6 @@
     <t>Lions</t>
   </si>
   <si>
-    <t>Titans</t>
-  </si>
-  <si>
-    <t>Texans</t>
-  </si>
-  <si>
     <t>Raiders</t>
   </si>
   <si>
@@ -128,31 +122,19 @@
     <t>Broncos</t>
   </si>
   <si>
-    <t>Cowboys</t>
-  </si>
-  <si>
     <t>49ers</t>
   </si>
   <si>
     <t>Ravens</t>
   </si>
   <si>
-    <t>Jets</t>
-  </si>
-  <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Bengals</t>
   </si>
   <si>
     <t>Jaguars</t>
   </si>
   <si>
     <t>Dolphins</t>
-  </si>
-  <si>
-    <t>Panthers</t>
   </si>
   <si>
     <t>Cardinals</t>
@@ -188,10 +170,16 @@
     <t>Chargers</t>
   </si>
   <si>
-    <t>6</t>
+    <t>Steelers</t>
   </si>
   <si>
-    <t>Packers, Steelers</t>
+    <t>Packers</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Bengals, Cowboys, Jets, Panthers, Texans, Titans</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1241,13 +1229,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1287,13 +1275,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1320,7 +1308,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Broncos at Chiefs (Game 1).</v>
+        <v>Pick a winner (V or H) for Jaguars at Saints (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1333,13 +1321,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1363,7 +1351,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Chiefs (Game 1).</v>
+        <v>Assign a weight to the Saints (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1376,13 +1364,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1419,13 +1407,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1462,13 +1450,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1492,7 +1480,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Cowboys at Chargers (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for 49ers at Vikings (Game 13) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1505,13 +1493,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1543,13 +1531,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1581,13 +1569,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1619,13 +1607,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1657,13 +1645,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1695,13 +1683,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1730,30 +1718,30 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35">
+    <row r="16" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="28" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="I16" s="18"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1768,30 +1756,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1812,13 +1800,13 @@
         <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1847,16 +1835,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1889,7 +1877,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 13 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1904,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1983,7 +1971,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1992,7 +1980,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2074,11 +2062,11 @@
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2142,11 +2130,11 @@
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 7 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D134FE-553B-4457-8AD4-11645E600428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAF3D2A-4588-4986-AA9F-E42B0689A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Bears</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Seahawks</t>
   </si>
   <si>
@@ -176,10 +173,28 @@
     <t>Packers</t>
   </si>
   <si>
-    <t>7</t>
+    <t>Texans</t>
   </si>
   <si>
-    <t>Bengals, Cowboys, Jets, Panthers, Texans, Titans</t>
+    <t>Panthers</t>
+  </si>
+  <si>
+    <t>Cowboys</t>
+  </si>
+  <si>
+    <t>Jets</t>
+  </si>
+  <si>
+    <t>Titans</t>
+  </si>
+  <si>
+    <t>Bengals</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1229,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1275,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1308,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jaguars at Saints (Game 1).</v>
+        <v>Pick a winner (V or H) for Buccaneers at Bills (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1321,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1351,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Saints (Game 1).</v>
+        <v>Assign a weight to the Bills (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1364,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1407,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1450,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1480,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for 49ers at Vikings (Game 13) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Raiders at Lions (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1493,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1531,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1569,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1607,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1645,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1683,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1718,30 +1733,30 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="str">
+    <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="I16" s="18"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1756,30 +1771,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="str">
+    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1794,30 +1809,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="str">
+    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1835,16 +1850,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1877,7 +1892,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 13 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1892,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1971,7 +1986,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1980,7 +1995,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2058,15 +2073,15 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2126,15 +2141,15 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 8 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAF3D2A-4588-4986-AA9F-E42B0689A3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6670312A-D122-4325-AFD7-F3E0EF6B0A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>at</t>
   </si>
@@ -95,9 +95,6 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Raiders</t>
   </si>
   <si>
@@ -119,19 +116,10 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>Broncos</t>
-  </si>
-  <si>
-    <t>49ers</t>
-  </si>
-  <si>
     <t>Ravens</t>
   </si>
   <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Jaguars</t>
   </si>
   <si>
     <t>Dolphins</t>
@@ -191,10 +179,13 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t>8</t>
+    <t/>
   </si>
   <si>
-    <t>None</t>
+    <t>9</t>
+  </si>
+  <si>
+    <t>49ers, Broncos, Jaguars, Lions</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1163,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1244,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1281,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1314,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Buccaneers at Bills (Game 1).</v>
+        <v>Pick a winner (V or H) for Titans at Steelers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1327,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1357,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bills (Game 1).</v>
+        <v>Assign a weight to the Steelers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1370,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1456,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1486,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Raiders at Lions (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Chargers at Jets (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1537,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1575,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1613,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1689,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1730,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1771,30 +1762,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1809,30 +1800,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
+    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1850,16 +1841,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1892,7 +1883,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 14 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1907,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1986,7 +1977,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1995,7 +1986,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2073,11 +2064,11 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2141,11 +2132,11 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 9 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6670312A-D122-4325-AFD7-F3E0EF6B0A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41876DC-71B7-4007-8B49-F28545B71B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,16 +101,7 @@
     <t>Vikings</t>
   </si>
   <si>
-    <t>Eagles</t>
-  </si>
-  <si>
-    <t>Rams</t>
-  </si>
-  <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Chiefs</t>
   </si>
   <si>
     <t>Giants</t>
@@ -120,9 +111,6 @@
   </si>
   <si>
     <t>Patriots</t>
-  </si>
-  <si>
-    <t>Dolphins</t>
   </si>
   <si>
     <t>Cardinals</t>
@@ -182,10 +170,22 @@
     <t/>
   </si>
   <si>
-    <t>9</t>
+    <t>49ers</t>
   </si>
   <si>
-    <t>49ers, Broncos, Jaguars, Lions</t>
+    <t>Jaguars</t>
+  </si>
+  <si>
+    <t>Lions</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Chiefs, Dolphins, Eagles, Rams</t>
   </si>
 </sst>
 </file>
@@ -1235,13 +1235,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1281,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Titans at Steelers (Game 1).</v>
+        <v>Pick a winner (V or H) for Panthers at Bears (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1327,13 +1327,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Steelers (Game 1).</v>
+        <v>Assign a weight to the Bears (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1370,13 +1370,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1413,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1456,13 +1456,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Chargers at Jets (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Broncos at Bills (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1499,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1537,13 +1537,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1575,13 +1575,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1613,13 +1613,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1651,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1689,13 +1689,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1730,13 +1730,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1768,13 +1768,13 @@
         <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1806,13 +1806,13 @@
         <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1844,13 +1844,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 10 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41876DC-71B7-4007-8B49-F28545B71B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598A8DA-A914-4368-8E3A-F94C3C23A0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,19 +110,7 @@
     <t>Ravens</t>
   </si>
   <si>
-    <t>Patriots</t>
-  </si>
-  <si>
     <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Colts</t>
-  </si>
-  <si>
-    <t>Falcons</t>
-  </si>
-  <si>
-    <t>Saints</t>
   </si>
   <si>
     <t>Commanders</t>
@@ -176,16 +164,28 @@
     <t>Jaguars</t>
   </si>
   <si>
-    <t>Lions</t>
-  </si>
-  <si>
     <t>Broncos</t>
   </si>
   <si>
-    <t>10</t>
+    <t>Detriot Lions</t>
   </si>
   <si>
-    <t>Chiefs, Dolphins, Eagles, Rams</t>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Rams</t>
+  </si>
+  <si>
+    <t>Eagles</t>
+  </si>
+  <si>
+    <t>Chiefs</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Colts, Falcons, Patriots, Saints</t>
   </si>
 </sst>
 </file>
@@ -1241,7 +1241,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1281,13 +1281,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1314,7 +1314,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Panthers at Bears (Game 1).</v>
+        <v>Pick a winner (V or H) for Bengals at Ravens (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1327,13 +1327,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Bears (Game 1).</v>
+        <v>Assign a weight to the Ravens (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1370,13 +1370,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1413,13 +1413,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1456,13 +1456,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Broncos at Bills (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Eagles at Chiefs (Game 14) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1499,13 +1499,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1537,13 +1537,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1575,7 +1575,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
@@ -1613,13 +1613,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1651,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1689,13 +1689,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1730,13 +1730,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1768,13 +1768,13 @@
         <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1806,13 +1806,13 @@
         <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1844,13 +1844,13 @@
         <v>14</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 11 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D598A8DA-A914-4368-8E3A-F94C3C23A0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67776DD4-CDBD-4017-A4E2-6BD66788CF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -155,9 +155,6 @@
     <t>Bengals</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>49ers</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
   </si>
   <si>
     <t>Broncos</t>
-  </si>
-  <si>
-    <t>Detriot Lions</t>
   </si>
   <si>
     <t>Dolphins</t>
@@ -182,10 +176,25 @@
     <t>Chiefs</t>
   </si>
   <si>
-    <t>11</t>
+    <t>Lions</t>
   </si>
   <si>
-    <t>Colts, Falcons, Patriots, Saints</t>
+    <t>Saints</t>
+  </si>
+  <si>
+    <t>Falcons</t>
+  </si>
+  <si>
+    <t>Colts</t>
+  </si>
+  <si>
+    <t>Patriots</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1235,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1281,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1314,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Bengals at Ravens (Game 1).</v>
+        <v>Pick a winner (V or H) for Packers at Lions (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1327,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1357,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Ravens (Game 1).</v>
+        <v>Assign a weight to the Lions (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1370,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1413,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1456,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1486,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Eagles at Chiefs (Game 14) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bears at Vikings (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1499,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1537,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1575,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1613,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1651,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1689,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1730,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1762,30 +1771,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="str">
+    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1800,30 +1809,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="str">
+    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1841,16 +1850,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1883,7 +1892,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 14 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1898,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1977,7 +1986,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1986,7 +1995,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2064,11 +2073,11 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
@@ -2132,11 +2141,11 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 12 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67776DD4-CDBD-4017-A4E2-6BD66788CF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823AB344-565A-40CF-B47F-E3B7141EB647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>at</t>
   </si>
@@ -95,28 +95,10 @@
     <t xml:space="preserve">Name:  </t>
   </si>
   <si>
-    <t>Raiders</t>
-  </si>
-  <si>
-    <t>Vikings</t>
-  </si>
-  <si>
-    <t>Bills</t>
-  </si>
-  <si>
-    <t>Giants</t>
-  </si>
-  <si>
-    <t>Ravens</t>
-  </si>
-  <si>
     <t>Cardinals</t>
   </si>
   <si>
     <t>Commanders</t>
-  </si>
-  <si>
-    <t>Bears</t>
   </si>
   <si>
     <t>Seahawks</t>
@@ -191,10 +173,13 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t>12</t>
+    <t/>
   </si>
   <si>
-    <t>None</t>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Bears, Bills, Giants, Raiders, Ravens, Vikings</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1244,13 +1229,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1275,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1308,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Packers at Lions (Game 1).</v>
+        <v>Pick a winner (V or H) for Seahawks at Cowboys (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1321,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1351,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Lions (Game 1).</v>
+        <v>Assign a weight to the Cowboys (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1385,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1407,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1450,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1480,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bears at Vikings (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Bengals at Jaguars (Game 13) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1493,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1531,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1569,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
@@ -1660,13 +1645,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1683,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1733,30 +1718,30 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35">
+    <row r="16" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v/>
       </c>
       <c r="C16" s="28" t="s">
         <v>44</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="I16" s="18"/>
-      <c r="AA16" s="1">
+      <c r="AA16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="AB16" s="1">
+        <v/>
+      </c>
+      <c r="AB16" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v/>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1771,30 +1756,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35">
+    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v>14</v>
+        <v/>
       </c>
       <c r="C17" s="28" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1">
+      <c r="AA17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="AB17" s="1">
+        <v/>
+      </c>
+      <c r="AB17" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v/>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1809,30 +1794,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35">
+    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35" t="str">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1">
+      <c r="AA18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="AB18" s="1">
+        <v/>
+      </c>
+      <c r="AB18" s="1" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v/>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1850,16 +1835,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1892,7 +1877,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 16 Total Points:  </v>
+        <v xml:space="preserve">Game 13 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1907,7 +1892,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1986,7 +1971,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1995,7 +1980,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2073,15 +2058,15 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2141,15 +2126,15 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v xml:space="preserve">1  </v>
+        <v/>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">2  </v>
+        <v/>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v xml:space="preserve">3  </v>
+        <v/>
       </c>
       <c r="F41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 13 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823AB344-565A-40CF-B47F-E3B7141EB647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AC657-2855-462C-B9FF-8DDA76543F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
   <si>
     <t>at</t>
   </si>
@@ -93,12 +93,6 @@
   </si>
   <si>
     <t xml:space="preserve">Name:  </t>
-  </si>
-  <si>
-    <t>Cardinals</t>
-  </si>
-  <si>
-    <t>Commanders</t>
   </si>
   <si>
     <t>Seahawks</t>
@@ -176,10 +170,28 @@
     <t/>
   </si>
   <si>
-    <t>13</t>
+    <t>Ravens</t>
   </si>
   <si>
-    <t>Bears, Bills, Giants, Raiders, Ravens, Vikings</t>
+    <t>Bears</t>
+  </si>
+  <si>
+    <t>Vikings</t>
+  </si>
+  <si>
+    <t>Raiders</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Giants</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Cardinals, Commanders</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1169,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1229,13 +1241,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1275,13 +1287,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1308,7 +1320,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Seahawks at Cowboys (Game 1).</v>
+        <v>Pick a winner (V or H) for Patriots at Steelers (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1321,13 +1333,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1351,7 +1363,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Cowboys (Game 1).</v>
+        <v>Assign a weight to the Steelers (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1364,13 +1376,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1407,13 +1419,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1450,13 +1462,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1480,7 +1492,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Bengals at Jaguars (Game 13) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Packers at Giants (Game 15) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1493,13 +1505,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1531,13 +1543,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1569,13 +1581,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1607,13 +1619,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1645,13 +1657,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1683,13 +1695,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1718,30 +1730,30 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="35" t="str">
+    <row r="16" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35">
         <f ca="1">IF(AND(ISTEXT($C16),$C16&lt;&gt;""),ROW($B16)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B16)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
       <c r="I16" s="18"/>
-      <c r="AA16" s="1" t="str">
+      <c r="AA16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB16" s="1" t="str">
+        <v>16</v>
+      </c>
+      <c r="AB16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>16</v>
       </c>
       <c r="AC16" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1756,30 +1768,30 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="str">
+    <row r="17" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="35">
         <f ca="1">IF(AND(ISTEXT($C17),$C17&lt;&gt;""),ROW($B17)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B17)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
       <c r="I17" s="18"/>
-      <c r="AA17" s="1" t="str">
+      <c r="AA17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB17" s="1" t="str">
+        <v>17</v>
+      </c>
+      <c r="AB17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>17</v>
       </c>
       <c r="AC17" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1800,13 +1812,13 @@
         <v/>
       </c>
       <c r="C18" s="28" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1835,16 +1847,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1877,7 +1889,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 13 Total Points:  </v>
+        <v xml:space="preserve">Game 15 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1892,7 +1904,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1971,7 +1983,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1980,7 +1992,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2062,11 +2074,11 @@
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,E39)&gt;0,COUNTIF($G4:$G19,E39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,F39)&gt;0,COUNTIF($G4:$G19,F39),-1)</f>
@@ -2130,11 +2142,11 @@
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">2  </v>
       </c>
       <c r="E41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v/>
+        <v xml:space="preserve">3  </v>
       </c>
       <c r="F41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 14 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72AC657-2855-462C-B9FF-8DDA76543F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004E412A-7EBF-4488-9E26-491939553C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="52">
   <si>
     <t>at</t>
   </si>
@@ -167,9 +167,6 @@
     <t>Patriots</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Ravens</t>
   </si>
   <si>
@@ -188,10 +185,16 @@
     <t>Giants</t>
   </si>
   <si>
-    <t>14</t>
+    <t>Cardinals</t>
   </si>
   <si>
-    <t>Cardinals, Commanders</t>
+    <t>Commanders</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1241,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1293,7 +1296,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1320,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Patriots at Steelers (Game 1).</v>
+        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1333,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1363,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Steelers (Game 1).</v>
+        <v>Assign a weight to the Raiders (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1376,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1419,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1462,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1492,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Packers at Giants (Game 15) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Steelers at Colts (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1505,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1543,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1581,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1619,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1657,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1695,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1736,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1774,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1806,30 +1809,30 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="str">
+    <row r="18" spans="2:42" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="35">
         <f ca="1">IF(AND(ISTEXT($C18),$C18&lt;&gt;""),ROW($B18)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B18)-ROW($B$4),0)),"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
       <c r="I18" s="18"/>
-      <c r="AA18" s="1" t="str">
+      <c r="AA18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="AB18" s="1" t="str">
+        <v>18</v>
+      </c>
+      <c r="AB18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v/>
+        <v>18</v>
       </c>
       <c r="AC18" s="1" t="str">
         <f t="shared" si="2"/>
@@ -1847,16 +1850,16 @@
     <row r="19" spans="2:42" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="36">
         <f ca="1">IF(AND(ISTEXT($C19),$C19&lt;&gt;""),ROW($B19)-ROW($B$3)-COUNTBLANK($C$4:OFFSET($C$4,ROW($B19)-ROW($B$4),0)),"")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1889,7 +1892,7 @@
       <c r="E20" s="14"/>
       <c r="F20" s="37" t="str">
         <f ca="1">IF(I2="","Pts:",CONCATENATE("Game ",B19," Total Points:  "))</f>
-        <v xml:space="preserve">Game 15 Total Points:  </v>
+        <v xml:space="preserve">Game 16 Total Points:  </v>
       </c>
       <c r="G20" s="38"/>
       <c r="I20" s="18"/>
@@ -1904,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>
@@ -1983,7 +1986,7 @@
       </c>
       <c r="D35" s="7">
         <f>16-(COUNTBLANK($C$4:$C$19))</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G35" s="1"/>
       <c r="AE35" s="1"/>
@@ -1992,7 +1995,7 @@
     <row r="36" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="2" t="str">
         <f ca="1">CONCATENATE("Weights not used:  ",$C$41,$D$41,$E$41,$F$41,$G$41,$H$41,$I$41,$J$41,$K$41,$L$41,$M$41,$N$41,$O$41,$P$41,$Q$41,$R$41)</f>
-        <v xml:space="preserve">Weights not used:  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
+        <v xml:space="preserve">Weights not used:  1  2  3  4  5  6  7  8  9  10  11  12  13  14  15  16  </v>
       </c>
       <c r="D36" s="5"/>
       <c r="G36" s="1"/>
@@ -2070,7 +2073,7 @@
     <row r="40" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,C39)&gt;0,COUNTIF($G4:$G19,C39),-1)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="1">
         <f ca="1">IF(COUNTIF((OFFSET($R$39,0,-($D$35)+1)):$R$39,D39)&gt;0,COUNTIF($G4:$G19,D39),-1)</f>
@@ -2138,7 +2141,7 @@
     <row r="41" spans="3:42" ht="20.100000000000001" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="str">
         <f t="shared" ref="C41:R41" ca="1" si="4">IF(C40=0,CONCATENATE(C39,"  "),"")</f>
-        <v/>
+        <v xml:space="preserve">1  </v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" ca="1" si="4"/>

</xml_diff>

<commit_message>
2023 Week 15 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004E412A-7EBF-4488-9E26-491939553C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F07C7C-8046-43E9-8A3E-5AB36F65D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,10 +191,10 @@
     <t>Commanders</t>
   </si>
   <si>
-    <t>15</t>
+    <t>None</t>
   </si>
   <si>
-    <t>None</t>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1172,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E1" s="51" t="s">
         <v>7</v>
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Chargers at Raiders (Game 1).</v>
+        <v>Pick a winner (V or H) for Saints at Rams (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Raiders (Game 1).</v>
+        <v>Assign a weight to the Rams (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Steelers at Colts (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Ravens at 49ers (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1777,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1815,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1853,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
@@ -1907,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E21" s="47"/>
       <c r="F21" s="47"/>

</xml_diff>

<commit_message>
2023 Week 16 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F07C7C-8046-43E9-8A3E-5AB36F65D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D05A76-E15C-40B3-A0BC-6EA3E9D5523E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>16</t>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Saints at Rams (Game 1).</v>
+        <v>Pick a winner (V or H) for Jets at Browns (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Rams (Game 1).</v>
+        <v>Assign a weight to the Browns (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,7 +1465,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Ravens at 49ers (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Packers at Vikings (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,13 +1508,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22"/>
@@ -1546,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1777,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1815,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1853,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>

<commit_message>
2023 Week 17 Preliminary update.
</commit_message>
<xml_diff>
--- a/regular_season_inputs.xlsx
+++ b/regular_season_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Football Pool\Web Pages\2023 Football Pool Page\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D05A76-E15C-40B3-A0BC-6EA3E9D5523E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B57D24-9D6F-4516-9BFD-8379C87E01B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
     <t>None</t>
   </si>
   <si>
-    <t>17</t>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1244,13 +1244,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -1290,13 +1290,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D5" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="22"/>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="AE5" s="2" t="str">
         <f ca="1">IF($AA$3&gt;0,CONCATENATE("Pick a winner (V or H) for ",OFFSET($C$4,$AA$3-ROW($B$4),0)," at ",OFFSET($E$4,$AA$3-ROW($B$4),0)," (Game ",OFFSET($B$4,$AA$3-ROW($B$4),0),")."),"")</f>
-        <v>Pick a winner (V or H) for Jets at Browns (Game 1).</v>
+        <v>Pick a winner (V or H) for Seahawks at Cardinals (Game 1).</v>
       </c>
       <c r="AP5" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G5=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP4,"")=ROW()-ROW($B$3),""," and "),IF($F5="V",$C5,$E5)," (Game ",$B5,")"),"")),"")</f>
@@ -1336,13 +1336,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F6" s="21"/>
       <c r="G6" s="22"/>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="AE6" s="2" t="str">
         <f ca="1">IF($AB$3&gt;0,CONCATENATE($AA$22," to the ",IF(OFFSET($F$4,$AB$3-ROW($B$4),0)="V",OFFSET($C$4,$AB$3-ROW($B$4),0),OFFSET($E$4,$AB$3-ROW($B$4),0))," (Game ",OFFSET($B$4,$AB$3-ROW($B$4),0),")."),"")</f>
-        <v>Assign a weight to the Browns (Game 1).</v>
+        <v>Assign a weight to the Cardinals (Game 1).</v>
       </c>
       <c r="AP6" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G6=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP5,"")=ROW()-ROW($B$3),""," and "),IF($F6="V",$C6,$E6)," (Game ",$B6,")"),"")),"")</f>
@@ -1379,13 +1379,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="22"/>
@@ -1422,13 +1422,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="22"/>
@@ -1465,13 +1465,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="21"/>
       <c r="G9" s="22"/>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="AE9" s="2" t="str">
         <f ca="1">IF(total_points="",CONCATENATE("Enter your Total Points Prediction for ",C19," at ",E19," (Game ",B19,") in cell ",ADDRESS(ROW(total_points),COLUMN(total_points),4),"."),"")</f>
-        <v>Enter your Total Points Prediction for Packers at Vikings (Game 16) in cell G20.</v>
+        <v>Enter your Total Points Prediction for Cowboys at Commanders (Game 16) in cell G20.</v>
       </c>
       <c r="AP9" s="2" t="str">
         <f ca="1">IF($AC$3&gt;0,(IF($G9=OFFSET($G$4,$AC$3-ROW($B$4),0),CONCATENATE(IF(COUNTIF($AP$3:$AP8,"")=ROW()-ROW($B$3),""," and "),IF($F9="V",$C9,$E9)," (Game ",$B9,")"),"")),"")</f>
@@ -1508,7 +1508,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D10" s="29" t="s">
         <v>0</v>
@@ -1546,13 +1546,13 @@
         <v>8</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
@@ -1584,13 +1584,13 @@
         <v>9</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13" s="21"/>
       <c r="G13" s="22"/>
@@ -1660,13 +1660,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D14" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="22"/>
@@ -1698,13 +1698,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D15" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="F15" s="21"/>
       <c r="G15" s="22"/>
@@ -1739,13 +1739,13 @@
         <v>13</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D16" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="22"/>
@@ -1777,13 +1777,13 @@
         <v>14</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="22"/>
@@ -1815,13 +1815,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F18" s="21"/>
       <c r="G18" s="22"/>
@@ -1853,13 +1853,13 @@
         <v>16</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D19" s="32" t="s">
         <v>0</v>
       </c>
       <c r="E19" s="33" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>

</xml_diff>